<commit_message>
[#34] Foldable feature minor fixes in doc - replacin b by B in Buttons description
</commit_message>
<xml_diff>
--- a/example/cz_app/xls/E_CZ_T2C_authoring.xlsx
+++ b/example/cz_app/xls/E_CZ_T2C_authoring.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="19126"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="19226"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CFF85B04-841C-4589-85B5-D45B617A00A5}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A5D2350E-E004-4076-9D23-BCFD2C34DFC9}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="15336" windowHeight="3744" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Tutorial" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="179016" concurrentCalc="0"/>
+  <calcPr calcId="179016"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="194" uniqueCount="181">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="199" uniqueCount="186">
   <si>
     <r>
       <rPr>
@@ -590,9 +590,6 @@
     <t>//  Příklad:</t>
   </si>
   <si>
-    <t xml:space="preserve">Toto jsou vaše možnosti: %%b teď byl převezen=teď byl převezen do nemocnice;brzy propustí= pacienta brzy propustí z nemocnice </t>
-  </si>
-  <si>
     <t>Jaké jsou možnosti</t>
   </si>
   <si>
@@ -765,6 +762,38 @@
   </si>
   <si>
     <t>//  'true &amp;&amp;' je docasna oprava chyby v detekci podmínky, po jejím opravení nebude potřeba</t>
+  </si>
+  <si>
+    <t>foldable</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">// </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="238"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Foldables</t>
+    </r>
+  </si>
+  <si>
+    <t>// Foldables  (rozbalovací texty) se na yačátku yobrayí ve své krátké variantě (npříklad jen jako titulek) a pokud na ně uživatel klikne, krátká forma se nahradí  dlouhou</t>
+  </si>
+  <si>
+    <t>roybalovací text</t>
+  </si>
+  <si>
+    <t>Příklad %%Ftitulek=dlouhá forma textu; druhý titulek= a velmi dlouhá forma druhého titulku</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Toto jsou vaše možnosti: %%B teď byl převezen=teď byl převezen do nemocnice;brzy propustí= pacienta brzy propustí z nemocnice </t>
   </si>
 </sst>
 </file>
@@ -1192,10 +1221,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D208"/>
+  <dimension ref="A1:D213"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A120" workbookViewId="0">
-      <selection activeCell="A141" sqref="A141"/>
+    <sheetView tabSelected="1" topLeftCell="A198" workbookViewId="0">
+      <selection activeCell="B198" sqref="B198"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1217,7 +1246,7 @@
     </row>
     <row r="4" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.3">
@@ -1227,7 +1256,7 @@
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.3">
@@ -1288,7 +1317,7 @@
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A19" s="1" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.3">
@@ -1348,7 +1377,7 @@
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.3">
@@ -1486,10 +1515,10 @@
         <v>44</v>
       </c>
       <c r="C55" s="8" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="D55" s="8" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
     </row>
     <row r="56" spans="1:4" x14ac:dyDescent="0.3">
@@ -1500,7 +1529,7 @@
     </row>
     <row r="57" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A57" s="8" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="B57" s="8"/>
       <c r="C57" s="8"/>
@@ -1508,7 +1537,7 @@
     </row>
     <row r="58" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A58" s="8" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="B58" s="9" t="s">
         <v>45</v>
@@ -1524,7 +1553,7 @@
     </row>
     <row r="60" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A60" s="12" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="B60" s="9" t="s">
         <v>46</v>
@@ -1533,7 +1562,7 @@
         <v>47</v>
       </c>
       <c r="D60" s="8" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
     </row>
     <row r="61" spans="1:4" x14ac:dyDescent="0.3">
@@ -1544,7 +1573,7 @@
     </row>
     <row r="62" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A62" s="8" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="B62" s="8"/>
       <c r="C62" s="8"/>
@@ -1578,7 +1607,7 @@
     </row>
     <row r="67" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A67" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
     </row>
     <row r="68" spans="1:4" s="17" customFormat="1" x14ac:dyDescent="0.3">
@@ -1588,7 +1617,7 @@
     </row>
     <row r="69" spans="1:4" s="17" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A69" s="16" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
     </row>
     <row r="70" spans="1:4" x14ac:dyDescent="0.3">
@@ -1942,7 +1971,7 @@
     </row>
     <row r="129" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A129" s="8" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="B129" s="8"/>
       <c r="C129" s="8"/>
@@ -2002,7 +2031,7 @@
     </row>
     <row r="141" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A141" s="8" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="B141" s="8" t="s">
         <v>105</v>
@@ -2012,7 +2041,7 @@
     </row>
     <row r="142" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A142" s="8" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="B142" s="8" t="s">
         <v>106</v>
@@ -2022,7 +2051,7 @@
     </row>
     <row r="143" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A143" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
     </row>
     <row r="144" spans="1:4" x14ac:dyDescent="0.3">
@@ -2184,17 +2213,17 @@
     </row>
     <row r="171" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A171" s="16" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
     </row>
     <row r="172" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A172" s="16" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
     </row>
     <row r="173" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A173" s="16" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
     </row>
     <row r="174" spans="1:4" x14ac:dyDescent="0.3">
@@ -2259,7 +2288,7 @@
     </row>
     <row r="185" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A185" s="16" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
     </row>
     <row r="186" spans="1:4" x14ac:dyDescent="0.3">
@@ -2277,10 +2306,10 @@
     </row>
     <row r="189" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A189" s="8" t="s">
+        <v>164</v>
+      </c>
+      <c r="B189" s="8" t="s">
         <v>165</v>
-      </c>
-      <c r="B189" s="8" t="s">
-        <v>166</v>
       </c>
       <c r="C189" s="8"/>
       <c r="D189" s="8"/>
@@ -2293,10 +2322,10 @@
     </row>
     <row r="191" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A191" s="15" t="s">
+        <v>166</v>
+      </c>
+      <c r="B191" s="15" t="s">
         <v>167</v>
-      </c>
-      <c r="B191" s="15" t="s">
-        <v>168</v>
       </c>
       <c r="C191" s="15"/>
       <c r="D191" s="15"/>
@@ -2317,7 +2346,7 @@
     </row>
     <row r="195" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A195" s="16" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
     </row>
     <row r="196" spans="1:2" s="17" customFormat="1" x14ac:dyDescent="0.3">
@@ -2332,10 +2361,10 @@
     </row>
     <row r="198" spans="1:2" s="15" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A198" s="15" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="B198" s="15" t="s">
-        <v>144</v>
+        <v>185</v>
       </c>
     </row>
     <row r="199" spans="1:2" x14ac:dyDescent="0.3">
@@ -2343,48 +2372,74 @@
     </row>
     <row r="200" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A200" s="16" t="s">
-        <v>146</v>
+        <v>181</v>
       </c>
     </row>
     <row r="201" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A201" s="16" t="s">
-        <v>148</v>
+        <v>182</v>
       </c>
     </row>
     <row r="202" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A202" s="16" t="s">
-        <v>149</v>
+        <v>180</v>
+      </c>
+      <c r="B202" t="s">
+        <v>184</v>
       </c>
     </row>
     <row r="203" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A203" s="16" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="204" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A204" s="16"/>
+    </row>
+    <row r="205" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A205" s="16" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="206" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A206" s="16" t="s">
         <v>147</v>
       </c>
     </row>
-    <row r="204" spans="1:2" s="15" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A204" s="15" t="s">
-        <v>159</v>
-      </c>
-      <c r="B204" s="15" t="s">
+    <row r="207" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A207" s="16" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="208" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A208" s="16" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="209" spans="1:2" s="15" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A209" s="15" t="s">
+        <v>158</v>
+      </c>
+      <c r="B209" s="15" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="210" spans="1:2" s="15" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="211" spans="1:2" s="15" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A211" s="15" t="s">
         <v>150</v>
       </c>
     </row>
-    <row r="205" spans="1:2" s="15" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="206" spans="1:2" s="15" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A206" s="15" t="s">
+    <row r="212" spans="1:2" s="15" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A212" s="15" t="s">
         <v>151</v>
       </c>
-    </row>
-    <row r="207" spans="1:2" s="15" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A207" s="15" t="s">
+      <c r="B212" s="15" t="s">
         <v>152</v>
       </c>
-      <c r="B207" s="15" t="s">
-        <v>153</v>
-      </c>
-    </row>
-    <row r="208" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A208" s="16"/>
+    </row>
+    <row r="213" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A213" s="16"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
reflecting the feedback - replaced typos in code and doc, adding description to english version of doc
</commit_message>
<xml_diff>
--- a/example/cz_app/xls/E_CZ_T2C_authoring.xlsx
+++ b/example/cz_app/xls/E_CZ_T2C_authoring.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="19226"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A5D2350E-E004-4076-9D23-BCFD2C34DFC9}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AE32DBF1-6FC4-48DD-9150-0CFCB42D1FD1}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="15336" windowHeight="3744" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -584,9 +584,6 @@
     <t>Mám se úžasně.%%4 úžasně.</t>
   </si>
   <si>
-    <t>//  Tlačítka se zapisují do výstupu (sloupec B) zápisem %%b jmeno_tlacitka_A=odpovídající text;jmeno_tlacitka_B=odpovídající text pro B</t>
-  </si>
-  <si>
     <t>//  Příklad:</t>
   </si>
   <si>
@@ -784,16 +781,19 @@
     </r>
   </si>
   <si>
-    <t>// Foldables  (rozbalovací texty) se na yačátku yobrayí ve své krátké variantě (npříklad jen jako titulek) a pokud na ně uživatel klikne, krátká forma se nahradí  dlouhou</t>
-  </si>
-  <si>
-    <t>roybalovací text</t>
-  </si>
-  <si>
     <t>Příklad %%Ftitulek=dlouhá forma textu; druhý titulek= a velmi dlouhá forma druhého titulku</t>
   </si>
   <si>
     <t xml:space="preserve">Toto jsou vaše možnosti: %%B teď byl převezen=teď byl převezen do nemocnice;brzy propustí= pacienta brzy propustí z nemocnice </t>
+  </si>
+  <si>
+    <t>// Foldables (rozbalovací texty) je vlastnost specifická pro použití s clientv2.  Foldables  se na začátku zobrazí ve své krátké variantě (například jen jako titulek) a pokud na ně uživatel klikne, krátká forma se nahradí  dlouhou</t>
+  </si>
+  <si>
+    <t>// Přidávání tlačítek je vlastnost specifická pro použití s clientv2. Tlačítka se zapisují do výstupu (sloupec B) zápisem %%b jmeno_tlacitka_A=odpovídající text;jmeno_tlacitka_B=odpovídající text pro B</t>
+  </si>
+  <si>
+    <t>rozbalovací text</t>
   </si>
 </sst>
 </file>
@@ -1223,8 +1223,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:D213"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A198" workbookViewId="0">
-      <selection activeCell="B198" sqref="B198"/>
+    <sheetView tabSelected="1" topLeftCell="A195" workbookViewId="0">
+      <selection activeCell="A203" sqref="A203"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1246,7 +1246,7 @@
     </row>
     <row r="4" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.3">
@@ -1256,7 +1256,7 @@
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.3">
@@ -1317,7 +1317,7 @@
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A19" s="1" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.3">
@@ -1377,7 +1377,7 @@
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.3">
@@ -1515,10 +1515,10 @@
         <v>44</v>
       </c>
       <c r="C55" s="8" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="D55" s="8" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
     </row>
     <row r="56" spans="1:4" x14ac:dyDescent="0.3">
@@ -1529,7 +1529,7 @@
     </row>
     <row r="57" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A57" s="8" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="B57" s="8"/>
       <c r="C57" s="8"/>
@@ -1537,7 +1537,7 @@
     </row>
     <row r="58" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A58" s="8" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="B58" s="9" t="s">
         <v>45</v>
@@ -1553,7 +1553,7 @@
     </row>
     <row r="60" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A60" s="12" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="B60" s="9" t="s">
         <v>46</v>
@@ -1562,7 +1562,7 @@
         <v>47</v>
       </c>
       <c r="D60" s="8" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
     </row>
     <row r="61" spans="1:4" x14ac:dyDescent="0.3">
@@ -1573,7 +1573,7 @@
     </row>
     <row r="62" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A62" s="8" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="B62" s="8"/>
       <c r="C62" s="8"/>
@@ -1607,7 +1607,7 @@
     </row>
     <row r="67" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A67" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
     </row>
     <row r="68" spans="1:4" s="17" customFormat="1" x14ac:dyDescent="0.3">
@@ -1617,7 +1617,7 @@
     </row>
     <row r="69" spans="1:4" s="17" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A69" s="16" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
     </row>
     <row r="70" spans="1:4" x14ac:dyDescent="0.3">
@@ -1971,7 +1971,7 @@
     </row>
     <row r="129" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A129" s="8" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="B129" s="8"/>
       <c r="C129" s="8"/>
@@ -2031,7 +2031,7 @@
     </row>
     <row r="141" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A141" s="8" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="B141" s="8" t="s">
         <v>105</v>
@@ -2041,7 +2041,7 @@
     </row>
     <row r="142" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A142" s="8" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="B142" s="8" t="s">
         <v>106</v>
@@ -2051,7 +2051,7 @@
     </row>
     <row r="143" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A143" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
     </row>
     <row r="144" spans="1:4" x14ac:dyDescent="0.3">
@@ -2213,17 +2213,17 @@
     </row>
     <row r="171" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A171" s="16" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
     </row>
     <row r="172" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A172" s="16" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
     </row>
     <row r="173" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A173" s="16" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
     </row>
     <row r="174" spans="1:4" x14ac:dyDescent="0.3">
@@ -2288,7 +2288,7 @@
     </row>
     <row r="185" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A185" s="16" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
     </row>
     <row r="186" spans="1:4" x14ac:dyDescent="0.3">
@@ -2306,10 +2306,10 @@
     </row>
     <row r="189" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A189" s="8" t="s">
+        <v>163</v>
+      </c>
+      <c r="B189" s="8" t="s">
         <v>164</v>
-      </c>
-      <c r="B189" s="8" t="s">
-        <v>165</v>
       </c>
       <c r="C189" s="8"/>
       <c r="D189" s="8"/>
@@ -2322,10 +2322,10 @@
     </row>
     <row r="191" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A191" s="15" t="s">
+        <v>165</v>
+      </c>
+      <c r="B191" s="15" t="s">
         <v>166</v>
-      </c>
-      <c r="B191" s="15" t="s">
-        <v>167</v>
       </c>
       <c r="C191" s="15"/>
       <c r="D191" s="15"/>
@@ -2346,25 +2346,25 @@
     </row>
     <row r="195" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A195" s="16" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
     </row>
     <row r="196" spans="1:2" s="17" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A196" s="16" t="s">
-        <v>142</v>
+        <v>184</v>
       </c>
     </row>
     <row r="197" spans="1:2" s="17" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A197" s="16" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
     </row>
     <row r="198" spans="1:2" s="15" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A198" s="15" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="B198" s="15" t="s">
-        <v>185</v>
+        <v>182</v>
       </c>
     </row>
     <row r="199" spans="1:2" x14ac:dyDescent="0.3">
@@ -2372,25 +2372,25 @@
     </row>
     <row r="200" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A200" s="16" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
     </row>
     <row r="201" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A201" s="16" t="s">
-        <v>182</v>
+        <v>183</v>
       </c>
     </row>
     <row r="202" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A202" s="16" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="B202" t="s">
-        <v>184</v>
+        <v>181</v>
       </c>
     </row>
     <row r="203" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A203" s="16" t="s">
-        <v>183</v>
+        <v>185</v>
       </c>
     </row>
     <row r="204" spans="1:2" x14ac:dyDescent="0.3">
@@ -2398,44 +2398,44 @@
     </row>
     <row r="205" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A205" s="16" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
     </row>
     <row r="206" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A206" s="16" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
     </row>
     <row r="207" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A207" s="16" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
     </row>
     <row r="208" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A208" s="16" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
     </row>
     <row r="209" spans="1:2" s="15" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A209" s="15" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="B209" s="15" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
     </row>
     <row r="210" spans="1:2" s="15" customFormat="1" x14ac:dyDescent="0.3"/>
     <row r="211" spans="1:2" s="15" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A211" s="15" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
     </row>
     <row r="212" spans="1:2" s="15" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A212" s="15" t="s">
+        <v>150</v>
+      </c>
+      <c r="B212" s="15" t="s">
         <v>151</v>
-      </c>
-      <c r="B212" s="15" t="s">
-        <v>152</v>
       </c>
     </row>
     <row r="213" spans="1:2" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
wording change foldables-rozbalovaci texty
</commit_message>
<xml_diff>
--- a/example/cz_app/xls/E_CZ_T2C_authoring.xlsx
+++ b/example/cz_app/xls/E_CZ_T2C_authoring.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="19226"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AE32DBF1-6FC4-48DD-9150-0CFCB42D1FD1}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D9374CFA-8F1A-4827-B946-3EA05AA9AD0B}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="15336" windowHeight="3744" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -764,8 +764,23 @@
     <t>foldable</t>
   </si>
   <si>
-    <r>
-      <t xml:space="preserve">// </t>
+    <t>Příklad %%Ftitulek=dlouhá forma textu; druhý titulek= a velmi dlouhá forma druhého titulku</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Toto jsou vaše možnosti: %%B teď byl převezen=teď byl převezen do nemocnice;brzy propustí= pacienta brzy propustí z nemocnice </t>
+  </si>
+  <si>
+    <t>// Foldables (rozbalovací texty) je vlastnost specifická pro použití s clientv2.  Foldables  se na začátku zobrazí ve své krátké variantě (například jen jako titulek) a pokud na ně uživatel klikne, krátká forma se nahradí  dlouhou</t>
+  </si>
+  <si>
+    <t>// Přidávání tlačítek je vlastnost specifická pro použití s clientv2. Tlačítka se zapisují do výstupu (sloupec B) zápisem %%b jmeno_tlacitka_A=odpovídající text;jmeno_tlacitka_B=odpovídající text pro B</t>
+  </si>
+  <si>
+    <t>rozbalovací text</t>
+  </si>
+  <si>
+    <r>
+      <t>//</t>
     </r>
     <r>
       <rPr>
@@ -777,23 +792,8 @@
         <charset val="238"/>
         <scheme val="minor"/>
       </rPr>
-      <t>Foldables</t>
-    </r>
-  </si>
-  <si>
-    <t>Příklad %%Ftitulek=dlouhá forma textu; druhý titulek= a velmi dlouhá forma druhého titulku</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Toto jsou vaše možnosti: %%B teď byl převezen=teď byl převezen do nemocnice;brzy propustí= pacienta brzy propustí z nemocnice </t>
-  </si>
-  <si>
-    <t>// Foldables (rozbalovací texty) je vlastnost specifická pro použití s clientv2.  Foldables  se na začátku zobrazí ve své krátké variantě (například jen jako titulek) a pokud na ně uživatel klikne, krátká forma se nahradí  dlouhou</t>
-  </si>
-  <si>
-    <t>// Přidávání tlačítek je vlastnost specifická pro použití s clientv2. Tlačítka se zapisují do výstupu (sloupec B) zápisem %%b jmeno_tlacitka_A=odpovídající text;jmeno_tlacitka_B=odpovídající text pro B</t>
-  </si>
-  <si>
-    <t>rozbalovací text</t>
+      <t xml:space="preserve"> Rozbalovací texty (Foldables)</t>
+    </r>
   </si>
 </sst>
 </file>
@@ -1223,8 +1223,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:D213"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A195" workbookViewId="0">
-      <selection activeCell="A203" sqref="A203"/>
+    <sheetView tabSelected="1" topLeftCell="A190" workbookViewId="0">
+      <selection activeCell="A200" sqref="A200"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2351,7 +2351,7 @@
     </row>
     <row r="196" spans="1:2" s="17" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A196" s="16" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
     </row>
     <row r="197" spans="1:2" s="17" customFormat="1" x14ac:dyDescent="0.3">
@@ -2364,7 +2364,7 @@
         <v>143</v>
       </c>
       <c r="B198" s="15" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
     </row>
     <row r="199" spans="1:2" x14ac:dyDescent="0.3">
@@ -2372,12 +2372,12 @@
     </row>
     <row r="200" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A200" s="16" t="s">
-        <v>180</v>
+        <v>185</v>
       </c>
     </row>
     <row r="201" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A201" s="16" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
     </row>
     <row r="202" spans="1:2" x14ac:dyDescent="0.3">
@@ -2385,12 +2385,12 @@
         <v>179</v>
       </c>
       <c r="B202" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
     </row>
     <row r="203" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A203" s="16" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
     </row>
     <row r="204" spans="1:2" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
minor formating changes in doc
</commit_message>
<xml_diff>
--- a/example/cz_app/xls/E_CZ_T2C_authoring.xlsx
+++ b/example/cz_app/xls/E_CZ_T2C_authoring.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="19226"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B65A4292-A5E5-4540-BE96-38390FEAF8A9}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DD5C6154-A5DB-48B2-AB5D-6641ED2C93AC}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="15336" windowHeight="3744" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1223,8 +1223,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:D213"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A184" workbookViewId="0">
-      <selection activeCell="A195" sqref="A195"/>
+    <sheetView tabSelected="1" topLeftCell="A167" workbookViewId="0">
+      <selection activeCell="C208" sqref="C208"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2359,13 +2359,15 @@
         <v>142</v>
       </c>
     </row>
-    <row r="198" spans="1:4" s="15" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="198" spans="1:4" s="16" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A198" s="15" t="s">
         <v>143</v>
       </c>
       <c r="B198" s="15" t="s">
         <v>180</v>
       </c>
+      <c r="C198" s="15"/>
+      <c r="D198" s="15"/>
     </row>
     <row r="199" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A199" s="16"/>
@@ -2421,29 +2423,41 @@
         <v>145</v>
       </c>
     </row>
-    <row r="209" spans="1:2" s="15" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="209" spans="1:4" s="16" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A209" s="15" t="s">
         <v>156</v>
       </c>
       <c r="B209" s="15" t="s">
         <v>148</v>
       </c>
-    </row>
-    <row r="210" spans="1:2" s="15" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="211" spans="1:2" s="15" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="C209" s="15"/>
+      <c r="D209" s="15"/>
+    </row>
+    <row r="210" spans="1:4" s="16" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A210" s="15"/>
+      <c r="B210" s="15"/>
+      <c r="C210" s="15"/>
+      <c r="D210" s="15"/>
+    </row>
+    <row r="211" spans="1:4" s="16" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A211" s="15" t="s">
         <v>149</v>
       </c>
-    </row>
-    <row r="212" spans="1:2" s="15" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="B211" s="15"/>
+      <c r="C211" s="15"/>
+      <c r="D211" s="15"/>
+    </row>
+    <row r="212" spans="1:4" s="16" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A212" s="15" t="s">
         <v>150</v>
       </c>
       <c r="B212" s="15" t="s">
         <v>151</v>
       </c>
-    </row>
-    <row r="213" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C212" s="15"/>
+      <c r="D212" s="15"/>
+    </row>
+    <row r="213" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A213" s="16"/>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
[#52] HTML support in T2C
</commit_message>
<xml_diff>
--- a/example/cz_app/xls/E_CZ_T2C_authoring.xlsx
+++ b/example/cz_app/xls/E_CZ_T2C_authoring.xlsx
@@ -1,9 +1,9 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="19226"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="19330"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DD5C6154-A5DB-48B2-AB5D-6641ED2C93AC}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E39B593A-8646-4983-9D89-30C041FD2425}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="15336" windowHeight="3744" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="199" uniqueCount="186">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="207" uniqueCount="194">
   <si>
     <r>
       <rPr>
@@ -645,9 +645,6 @@
     </r>
   </si>
   <si>
-    <t xml:space="preserve">// Druhý sloupec B je používín pro zápis výstupu. Tabulkový formát zápisu podporuje mimo jednoduchého textového zápisu i možnost zápisu výstupů pro více kanálů zároveň. </t>
-  </si>
-  <si>
     <t xml:space="preserve">// Výstupy do dalších kanálů jsou uvedeny znaky %%n, kde n je číslo kanálu. Význam kanálů závisí na interpretaci užívaným klientem. </t>
   </si>
   <si>
@@ -794,6 +791,33 @@
   </si>
   <si>
     <t>// Bot reaguje textem "Mám se úžasně" a zároveň řekne  "Úžasně"</t>
+  </si>
+  <si>
+    <t>HTML</t>
+  </si>
+  <si>
+    <t>Prvy a &lt;br&gt; druhý řádek, nový &lt;p&gt; odstavec a &lt;h1&gt;nadpis&lt;/h1&gt;</t>
+  </si>
+  <si>
+    <t>Prvy a &amp;lt;br&amp;gt; druhý řádek, nový &amp;lt;p&amp;gt; odstavec a &amp;lt;h1&amp;gt;nadpis&amp;lt;/h1&amp;gt;</t>
+  </si>
+  <si>
+    <t>// kde: Prvy a &amp;lt;br&amp;gt; druhý řádek… odpovida: Prvy a &lt;br&gt; druhý řádek, nový &lt;p&gt; odstavec a &lt;h1&gt;nadpis&lt;/h1&gt;</t>
+  </si>
+  <si>
+    <t>HTMLEncoded</t>
+  </si>
+  <si>
+    <t xml:space="preserve">// Výstup je uvedený ve sloupci B. Může obsahovat i HTML značky. Defaultní klient (clientv2) HTML formát podporuje. </t>
+  </si>
+  <si>
+    <t>// (text je XML escapován při převodu do XML, znaky  &lt; &gt;"'' jsou nahrazeny přepisem (např.   &lt;  se stane &amp;lt). Zpětný převod je proveden při převodu do json formatu)</t>
+  </si>
+  <si>
+    <t>// Pokud potřebujete zobrazit  výše uvedené znaky bez jejich interprace jako HTML, je nutné tyto znaky zvlášť escapovat (např. s využitím např. https://www.freeformatter.com/xml-escape.html)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">// Tabulkový formát zápisu podporuje mimo jednoduchého textového zápisu i možnost zápisu výstupů pro více kanálů zároveň. </t>
   </si>
 </sst>
 </file>
@@ -1221,10 +1245,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D213"/>
+  <dimension ref="A1:D222"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A167" workbookViewId="0">
-      <selection activeCell="C208" sqref="C208"/>
+    <sheetView tabSelected="1" topLeftCell="A162" workbookViewId="0">
+      <selection activeCell="A181" sqref="A181"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1246,7 +1270,7 @@
     </row>
     <row r="4" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.3">
@@ -1256,7 +1280,7 @@
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.3">
@@ -1317,7 +1341,7 @@
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A19" s="1" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.3">
@@ -1377,7 +1401,7 @@
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.3">
@@ -1515,10 +1539,10 @@
         <v>44</v>
       </c>
       <c r="C55" s="8" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="D55" s="8" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
     </row>
     <row r="56" spans="1:4" x14ac:dyDescent="0.3">
@@ -1529,7 +1553,7 @@
     </row>
     <row r="57" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A57" s="8" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="B57" s="8"/>
       <c r="C57" s="8"/>
@@ -1537,7 +1561,7 @@
     </row>
     <row r="58" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A58" s="8" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="B58" s="9" t="s">
         <v>45</v>
@@ -1553,7 +1577,7 @@
     </row>
     <row r="60" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A60" s="12" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="B60" s="9" t="s">
         <v>46</v>
@@ -1562,7 +1586,7 @@
         <v>47</v>
       </c>
       <c r="D60" s="8" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
     </row>
     <row r="61" spans="1:4" x14ac:dyDescent="0.3">
@@ -1573,7 +1597,7 @@
     </row>
     <row r="62" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A62" s="8" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="B62" s="8"/>
       <c r="C62" s="8"/>
@@ -1607,7 +1631,7 @@
     </row>
     <row r="67" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A67" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
     </row>
     <row r="68" spans="1:4" s="17" customFormat="1" x14ac:dyDescent="0.3">
@@ -1617,7 +1641,7 @@
     </row>
     <row r="69" spans="1:4" s="17" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A69" s="16" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
     </row>
     <row r="70" spans="1:4" x14ac:dyDescent="0.3">
@@ -1971,7 +1995,7 @@
     </row>
     <row r="129" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A129" s="8" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="B129" s="8"/>
       <c r="C129" s="8"/>
@@ -2031,7 +2055,7 @@
     </row>
     <row r="141" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A141" s="8" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="B141" s="8" t="s">
         <v>105</v>
@@ -2041,7 +2065,7 @@
     </row>
     <row r="142" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A142" s="8" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="B142" s="8" t="s">
         <v>106</v>
@@ -2051,7 +2075,7 @@
     </row>
     <row r="143" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A143" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
     </row>
     <row r="144" spans="1:4" x14ac:dyDescent="0.3">
@@ -2218,247 +2242,289 @@
     </row>
     <row r="172" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A172" s="16" t="s">
-        <v>153</v>
+        <v>190</v>
       </c>
     </row>
     <row r="173" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A173" s="16" t="s">
-        <v>154</v>
+        <v>191</v>
       </c>
     </row>
     <row r="174" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A174" s="16" t="s">
-        <v>127</v>
-      </c>
-    </row>
-    <row r="175" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A175" s="16" t="s">
-        <v>130</v>
-      </c>
+      <c r="A174" s="8" t="s">
+        <v>185</v>
+      </c>
+      <c r="B174" s="8" t="s">
+        <v>186</v>
+      </c>
+      <c r="C174" s="8"/>
+      <c r="D174" s="8"/>
     </row>
     <row r="176" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A176" s="16" t="s">
-        <v>131</v>
-      </c>
-    </row>
-    <row r="177" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A177" s="16" t="s">
-        <v>132</v>
+        <v>192</v>
       </c>
     </row>
     <row r="178" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A178" s="16" t="s">
-        <v>133</v>
-      </c>
+      <c r="A178" s="8" t="s">
+        <v>189</v>
+      </c>
+      <c r="B178" s="8" t="s">
+        <v>187</v>
+      </c>
+      <c r="C178" s="8"/>
+      <c r="D178" s="8"/>
     </row>
     <row r="179" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A179" s="16" t="s">
-        <v>134</v>
-      </c>
-    </row>
-    <row r="180" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A180" s="16" t="s">
-        <v>135</v>
-      </c>
-    </row>
+        <v>188</v>
+      </c>
+      <c r="B179" s="16"/>
+    </row>
+    <row r="180" spans="1:4" s="16" customFormat="1" x14ac:dyDescent="0.3"/>
     <row r="181" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A181" s="16" t="s">
-        <v>136</v>
+        <v>193</v>
       </c>
     </row>
     <row r="182" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A182" s="16" t="s">
-        <v>137</v>
+        <v>153</v>
       </c>
     </row>
     <row r="183" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A183" s="16" t="s">
-        <v>139</v>
+        <v>127</v>
       </c>
     </row>
     <row r="184" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A184" s="8" t="s">
-        <v>140</v>
-      </c>
-      <c r="B184" s="8" t="s">
-        <v>141</v>
-      </c>
-      <c r="C184" s="8"/>
-      <c r="D184" s="8"/>
+      <c r="A184" s="16" t="s">
+        <v>130</v>
+      </c>
     </row>
     <row r="185" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A185" s="16" t="s">
-        <v>185</v>
+        <v>131</v>
       </c>
     </row>
     <row r="186" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A186" s="16"/>
+      <c r="A186" s="16" t="s">
+        <v>132</v>
+      </c>
     </row>
     <row r="187" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A187" s="16" t="s">
-        <v>128</v>
+        <v>133</v>
       </c>
     </row>
     <row r="188" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A188" s="16" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="189" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A189" s="16" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="190" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A190" s="16" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="191" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A191" s="16" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="192" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A192" s="16" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="193" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A193" s="8" t="s">
+        <v>140</v>
+      </c>
+      <c r="B193" s="8" t="s">
+        <v>141</v>
+      </c>
+      <c r="C193" s="8"/>
+      <c r="D193" s="8"/>
+    </row>
+    <row r="194" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A194" s="16" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="195" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A195" s="16"/>
+    </row>
+    <row r="196" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A196" s="16" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="197" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A197" s="16" t="s">
         <v>138</v>
       </c>
     </row>
-    <row r="189" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A189" s="8" t="s">
+    <row r="198" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A198" s="8" t="s">
+        <v>161</v>
+      </c>
+      <c r="B198" s="8" t="s">
         <v>162</v>
       </c>
-      <c r="B189" s="8" t="s">
+      <c r="C198" s="8"/>
+      <c r="D198" s="8"/>
+    </row>
+    <row r="199" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A199" s="15"/>
+      <c r="B199" s="15"/>
+      <c r="C199" s="15"/>
+      <c r="D199" s="15"/>
+    </row>
+    <row r="200" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A200" s="15" t="s">
         <v>163</v>
       </c>
-      <c r="C189" s="8"/>
-      <c r="D189" s="8"/>
-    </row>
-    <row r="190" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A190" s="15"/>
-      <c r="B190" s="15"/>
-      <c r="C190" s="15"/>
-      <c r="D190" s="15"/>
-    </row>
-    <row r="191" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A191" s="15" t="s">
+      <c r="B200" s="15" t="s">
         <v>164</v>
       </c>
-      <c r="B191" s="15" t="s">
-        <v>165</v>
-      </c>
-      <c r="C191" s="15"/>
-      <c r="D191" s="15"/>
-    </row>
-    <row r="192" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A192" s="15"/>
-      <c r="B192" s="15"/>
-      <c r="C192" s="15"/>
-      <c r="D192" s="15"/>
-    </row>
-    <row r="193" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A193" s="16" t="s">
+      <c r="C200" s="15"/>
+      <c r="D200" s="15"/>
+    </row>
+    <row r="201" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A201" s="15"/>
+      <c r="B201" s="15"/>
+      <c r="C201" s="15"/>
+      <c r="D201" s="15"/>
+    </row>
+    <row r="202" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A202" s="16" t="s">
         <v>129</v>
       </c>
     </row>
-    <row r="194" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A194" s="16"/>
-    </row>
-    <row r="195" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A195" s="16" t="s">
-        <v>155</v>
-      </c>
-    </row>
-    <row r="196" spans="1:4" s="17" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A196" s="16" t="s">
-        <v>182</v>
-      </c>
-    </row>
-    <row r="197" spans="1:4" s="17" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A197" s="16" t="s">
+    <row r="203" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A203" s="16"/>
+    </row>
+    <row r="204" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A204" s="16" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="205" spans="1:4" s="17" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A205" s="16" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="206" spans="1:4" s="17" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A206" s="16" t="s">
         <v>142</v>
       </c>
     </row>
-    <row r="198" spans="1:4" s="16" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A198" s="15" t="s">
+    <row r="207" spans="1:4" s="16" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A207" s="15" t="s">
         <v>143</v>
       </c>
-      <c r="B198" s="15" t="s">
+      <c r="B207" s="15" t="s">
+        <v>179</v>
+      </c>
+      <c r="C207" s="15"/>
+      <c r="D207" s="15"/>
+    </row>
+    <row r="208" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A208" s="16"/>
+    </row>
+    <row r="209" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A209" s="16" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="210" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A210" s="16" t="s">
         <v>180</v>
       </c>
-      <c r="C198" s="15"/>
-      <c r="D198" s="15"/>
-    </row>
-    <row r="199" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A199" s="16"/>
-    </row>
-    <row r="200" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A200" s="16" t="s">
-        <v>184</v>
-      </c>
-    </row>
-    <row r="201" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A201" s="16" t="s">
-        <v>181</v>
-      </c>
-    </row>
-    <row r="202" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A202" s="15" t="s">
+    </row>
+    <row r="211" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A211" s="15" t="s">
+        <v>177</v>
+      </c>
+      <c r="B211" s="15" t="s">
         <v>178</v>
       </c>
-      <c r="B202" s="15" t="s">
-        <v>179</v>
-      </c>
-      <c r="C202" s="15"/>
-      <c r="D202" s="15"/>
-    </row>
-    <row r="203" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A203" s="15" t="s">
-        <v>183</v>
-      </c>
-      <c r="B203" s="15"/>
-      <c r="C203" s="15"/>
-      <c r="D203" s="15"/>
-    </row>
-    <row r="204" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A204" s="16"/>
-    </row>
-    <row r="205" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A205" s="16" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="206" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A206" s="16" t="s">
-        <v>146</v>
-      </c>
-    </row>
-    <row r="207" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A207" s="16" t="s">
-        <v>147</v>
-      </c>
-    </row>
-    <row r="208" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A208" s="16" t="s">
-        <v>145</v>
-      </c>
-    </row>
-    <row r="209" spans="1:4" s="16" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A209" s="15" t="s">
-        <v>156</v>
-      </c>
-      <c r="B209" s="15" t="s">
-        <v>148</v>
-      </c>
-      <c r="C209" s="15"/>
-      <c r="D209" s="15"/>
-    </row>
-    <row r="210" spans="1:4" s="16" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A210" s="15"/>
-      <c r="B210" s="15"/>
-      <c r="C210" s="15"/>
-      <c r="D210" s="15"/>
-    </row>
-    <row r="211" spans="1:4" s="16" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A211" s="15" t="s">
-        <v>149</v>
-      </c>
-      <c r="B211" s="15"/>
       <c r="C211" s="15"/>
       <c r="D211" s="15"/>
     </row>
-    <row r="212" spans="1:4" s="16" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="212" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A212" s="15" t="s">
-        <v>150</v>
-      </c>
-      <c r="B212" s="15" t="s">
-        <v>151</v>
-      </c>
+        <v>182</v>
+      </c>
+      <c r="B212" s="15"/>
       <c r="C212" s="15"/>
       <c r="D212" s="15"/>
     </row>
     <row r="213" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A213" s="16"/>
+    </row>
+    <row r="214" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A214" s="16" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="215" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A215" s="16" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="216" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A216" s="16" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="217" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A217" s="16" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="218" spans="1:4" s="16" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A218" s="15" t="s">
+        <v>155</v>
+      </c>
+      <c r="B218" s="15" t="s">
+        <v>148</v>
+      </c>
+      <c r="C218" s="15"/>
+      <c r="D218" s="15"/>
+    </row>
+    <row r="219" spans="1:4" s="16" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A219" s="15"/>
+      <c r="B219" s="15"/>
+      <c r="C219" s="15"/>
+      <c r="D219" s="15"/>
+    </row>
+    <row r="220" spans="1:4" s="16" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A220" s="15" t="s">
+        <v>149</v>
+      </c>
+      <c r="B220" s="15"/>
+      <c r="C220" s="15"/>
+      <c r="D220" s="15"/>
+    </row>
+    <row r="221" spans="1:4" s="16" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A221" s="15" t="s">
+        <v>150</v>
+      </c>
+      <c r="B221" s="15" t="s">
+        <v>151</v>
+      </c>
+      <c r="C221" s="15"/>
+      <c r="D221" s="15"/>
+    </row>
+    <row r="222" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A222" s="16"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
[#161] support for enforced conditions introduced by #$ removed some unrelated files in examples
</commit_message>
<xml_diff>
--- a/example/cz_app/xls/E_CZ_T2C_authoring.xlsx
+++ b/example/cz_app/xls/E_CZ_T2C_authoring.xlsx
@@ -1,9 +1,9 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20730"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20827"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{937AF452-26FA-4EA0-B5D4-5E67BD31D24A}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B7BFDBBC-C859-4AED-B58C-854CD004EAE6}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="15336" windowHeight="3744" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="207" uniqueCount="194">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="211" uniqueCount="198">
   <si>
     <r>
       <rPr>
@@ -216,9 +216,6 @@
     </r>
   </si>
   <si>
-    <t>// Ne vždy je možné odpovídat na otázky bez znalosti kontextu, pokud chcete aby se některé kroky prováděli jen v návaznosti na sebe, můžete to popsat ve čtvrtém sloupečku  (D) uvedením jména sekce, která chování popisuje</t>
-  </si>
-  <si>
     <t xml:space="preserve">//   popis sekce pak začíná znakem : a stejným jménem </t>
   </si>
   <si>
@@ -304,9 +301,6 @@
   </si>
   <si>
     <t>Nechci</t>
-  </si>
-  <si>
-    <t>// Intent potom můžeme použít pro otázky, které se provedou bez ohledu na kontext, například:</t>
   </si>
   <si>
     <t>To jsem rád že souhlasíte</t>
@@ -746,15 +740,6 @@
     <t xml:space="preserve"> @KONCETINA</t>
   </si>
   <si>
-    <t xml:space="preserve"> true &amp;&amp; @KONCETINA:ruka </t>
-  </si>
-  <si>
-    <t xml:space="preserve"> true &amp;&amp; @KONCETINA:noha</t>
-  </si>
-  <si>
-    <t>//  'true &amp;&amp;' je docasna oprava chyby v detekci podmínky, po jejím opravení nebude potřeba</t>
-  </si>
-  <si>
     <t>foldable</t>
   </si>
   <si>
@@ -811,13 +796,40 @@
     <t xml:space="preserve">// Výstup je uvedený ve sloupci B. Může obsahovat i HTML značky. Defaultní klient (clientv2) HTML formát podporuje. </t>
   </si>
   <si>
-    <t>// (text je XML escapován při převodu do XML, znaky  &lt; &gt;"'' jsou nahrazeny přepisem (např.   &lt;  se stane &amp;lt). Zpětný převod je proveden při převodu do json formatu)</t>
-  </si>
-  <si>
     <t>// Pokud potřebujete zobrazit  výše uvedené znaky bez jejich interprace jako HTML, je nutné tyto znaky zvlášť escapovat (např. s využitím např. https://www.freeformatter.com/xml-escape.html)</t>
   </si>
   <si>
     <t xml:space="preserve">// Tabulkový formát zápisu podporuje mimo jednoduchého textového zápisu i možnost zápisu výstupů pro více kanálů zároveň. </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> @KONCETINA:ruka </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> @KONCETINA:noha</t>
+  </si>
+  <si>
+    <t>// Ne vždy je možné odpovídat na otázky bez znalosti kontextu, pokud chcete aby se některé kroky prováděly jen v návaznosti na sebe, můžete to popsat ve čtvrtém sloupečku  (D) uvedením jména sekce, která chování popisuje</t>
+  </si>
+  <si>
+    <t>// Intent potom můžeme použít pro otázky, které se provedou bez ohledu na kontext,</t>
+  </si>
+  <si>
+    <t>// (text je XML escapován při převodu do XML, znaky  &lt; &gt; jsou nahrazeny přepisem (např.   &lt;  se stane &amp;lt). Zpětný převod je proveden při převodu do json formatu)</t>
+  </si>
+  <si>
+    <t>Vítejte v našem ukázkové aplikaci</t>
+  </si>
+  <si>
+    <t>#$ welcome</t>
+  </si>
+  <si>
+    <t>// Text v levém sloupci musí být podmínka nebo text, nejde oba zapisy kombinovat.  Pokud jde o podmínku, je v levé části textu jen jedna, nelze psát několik podmínek pod sebou.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">// Pokud potřebujete vynutit, aby se text interpretoval jako podmínka, zahajte ho sekvencí znaků " #$ " (na konci je mezera). Tak jde například vynutit, aby se slova "welcome", "true", "false", "anything_else" interpretovala </t>
+  </si>
+  <si>
+    <t>// stejne, jak je chápe watson assistant, tedy aby se výstup zobrazil jen po startu konverzace (welcome), vždy (true), nikdy (false) nebo pokud nebyla splněna žádná předchozí podmínka(anything_else).</t>
   </si>
 </sst>
 </file>
@@ -1245,10 +1257,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D223"/>
+  <dimension ref="A1:D227"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A133" workbookViewId="0">
-      <selection activeCell="A145" sqref="A145"/>
+    <sheetView tabSelected="1" topLeftCell="A150" workbookViewId="0">
+      <selection activeCell="B172" sqref="B172"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1270,7 +1282,7 @@
     </row>
     <row r="4" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.3">
@@ -1280,7 +1292,7 @@
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.3">
@@ -1341,7 +1353,7 @@
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A19" s="1" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.3">
@@ -1401,7 +1413,7 @@
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.3">
@@ -1518,31 +1530,31 @@
     </row>
     <row r="51" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A51" t="s">
-        <v>40</v>
+        <v>190</v>
       </c>
     </row>
     <row r="52" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A52" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="53" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A53" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="55" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A55" s="8" t="s">
+        <v>42</v>
+      </c>
+      <c r="B55" s="8" t="s">
         <v>43</v>
       </c>
-      <c r="B55" s="8" t="s">
-        <v>44</v>
-      </c>
       <c r="C55" s="8" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="D55" s="8" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
     </row>
     <row r="56" spans="1:4" x14ac:dyDescent="0.3">
@@ -1553,7 +1565,7 @@
     </row>
     <row r="57" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A57" s="8" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="B57" s="8"/>
       <c r="C57" s="8"/>
@@ -1561,10 +1573,10 @@
     </row>
     <row r="58" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A58" s="8" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="B58" s="9" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C58" s="8"/>
       <c r="D58" s="8"/>
@@ -1577,16 +1589,16 @@
     </row>
     <row r="60" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A60" s="12" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="B60" s="9" t="s">
+        <v>45</v>
+      </c>
+      <c r="C60" s="8" t="s">
         <v>46</v>
       </c>
-      <c r="C60" s="8" t="s">
-        <v>47</v>
-      </c>
       <c r="D60" s="8" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
     </row>
     <row r="61" spans="1:4" x14ac:dyDescent="0.3">
@@ -1597,7 +1609,7 @@
     </row>
     <row r="62" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A62" s="8" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="B62" s="8"/>
       <c r="C62" s="8"/>
@@ -1605,10 +1617,10 @@
     </row>
     <row r="63" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A63" s="8" t="s">
+        <v>47</v>
+      </c>
+      <c r="B63" s="8" t="s">
         <v>48</v>
-      </c>
-      <c r="B63" s="8" t="s">
-        <v>49</v>
       </c>
       <c r="C63" s="8"/>
       <c r="D63" s="8"/>
@@ -1621,37 +1633,37 @@
     </row>
     <row r="65" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A65" s="8" t="s">
+        <v>49</v>
+      </c>
+      <c r="B65" s="8" t="s">
         <v>50</v>
-      </c>
-      <c r="B65" s="8" t="s">
-        <v>51</v>
       </c>
       <c r="C65" s="8"/>
       <c r="D65" s="8"/>
     </row>
     <row r="67" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A67" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
     </row>
     <row r="68" spans="1:4" s="17" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A68" s="16" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
     </row>
     <row r="69" spans="1:4" s="17" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A69" s="16" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
     </row>
     <row r="70" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A70" s="16" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
     </row>
     <row r="71" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A71" s="16" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
     </row>
     <row r="72" spans="1:4" x14ac:dyDescent="0.3">
@@ -1659,37 +1671,37 @@
     </row>
     <row r="73" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A73" s="13" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="74" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A74" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="75" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A75" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="76" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A76" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="77" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A77" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="78" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A78" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="80" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A80" s="9" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B80" s="9"/>
       <c r="C80" s="9"/>
@@ -1697,7 +1709,7 @@
     </row>
     <row r="81" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A81" s="9" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B81" s="9"/>
       <c r="C81" s="9"/>
@@ -1705,7 +1717,7 @@
     </row>
     <row r="82" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A82" s="9" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B82" s="9"/>
       <c r="C82" s="9"/>
@@ -1713,7 +1725,7 @@
     </row>
     <row r="83" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A83" s="9" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B83" s="9"/>
       <c r="C83" s="9"/>
@@ -1721,7 +1733,7 @@
     </row>
     <row r="84" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A84" s="9" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B84" s="9"/>
       <c r="C84" s="9"/>
@@ -1729,7 +1741,7 @@
     </row>
     <row r="85" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A85" s="9" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B85" s="9"/>
       <c r="C85" s="9"/>
@@ -1743,7 +1755,7 @@
     </row>
     <row r="87" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A87" s="8" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B87" s="8"/>
       <c r="C87" s="8"/>
@@ -1751,7 +1763,7 @@
     </row>
     <row r="88" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A88" s="8" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B88" s="8"/>
       <c r="C88" s="8"/>
@@ -1759,7 +1771,7 @@
     </row>
     <row r="89" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A89" s="8" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B89" s="8"/>
       <c r="C89" s="8"/>
@@ -1767,7 +1779,7 @@
     </row>
     <row r="90" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A90" s="8" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B90" s="8"/>
       <c r="C90" s="8"/>
@@ -1775,7 +1787,7 @@
     </row>
     <row r="91" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A91" s="8" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B91" s="8"/>
       <c r="C91" s="8"/>
@@ -1783,7 +1795,7 @@
     </row>
     <row r="92" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A92" s="8" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B92" s="8"/>
       <c r="C92" s="8"/>
@@ -1791,15 +1803,15 @@
     </row>
     <row r="94" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A94" t="s">
-        <v>70</v>
+        <v>191</v>
       </c>
     </row>
     <row r="96" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A96" s="8" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B96" s="8" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="C96" s="8"/>
       <c r="D96" s="8"/>
@@ -1812,34 +1824,34 @@
     </row>
     <row r="98" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A98" s="8" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B98" s="8" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="C98" s="8"/>
       <c r="D98" s="8"/>
     </row>
     <row r="100" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A100" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
     </row>
     <row r="102" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A102" s="8" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="B102" s="8" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="C102" s="8"/>
       <c r="D102" s="8" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
     </row>
     <row r="103" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A103" s="8" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="B103" s="8"/>
       <c r="C103" s="8"/>
@@ -1847,7 +1859,7 @@
     </row>
     <row r="104" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A104" s="8" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="B104" s="8"/>
       <c r="C104" s="8"/>
@@ -1861,7 +1873,7 @@
     </row>
     <row r="106" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A106" s="8" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="B106" s="8"/>
       <c r="C106" s="8"/>
@@ -1869,14 +1881,14 @@
     </row>
     <row r="107" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A107" s="8" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B107" s="8" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="C107" s="8"/>
       <c r="D107" s="8" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
     </row>
     <row r="108" spans="1:4" x14ac:dyDescent="0.3">
@@ -1887,10 +1899,10 @@
     </row>
     <row r="109" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A109" s="8" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B109" s="8" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="C109" s="8"/>
       <c r="D109" s="8"/>
@@ -1903,7 +1915,7 @@
     </row>
     <row r="111" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A111" s="8" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="B111" s="8"/>
       <c r="C111" s="8"/>
@@ -1911,10 +1923,10 @@
     </row>
     <row r="112" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A112" s="8" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B112" s="8" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="C112" s="8"/>
       <c r="D112" s="8"/>
@@ -1927,42 +1939,42 @@
     </row>
     <row r="114" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A114" s="8" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B114" s="8" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="C114" s="8"/>
       <c r="D114" s="8"/>
     </row>
     <row r="116" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A116" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
     </row>
     <row r="117" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A117" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
     </row>
     <row r="119" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A119" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
     </row>
     <row r="120" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A120" s="8" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="B120" s="8" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="C120" s="8"/>
       <c r="D120" s="8"/>
     </row>
     <row r="121" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A121" s="8" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="B121" s="8"/>
       <c r="C121" s="8"/>
@@ -1970,32 +1982,32 @@
     </row>
     <row r="123" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A123" s="13" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
     </row>
     <row r="124" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A124" s="14" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
     </row>
     <row r="125" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A125" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
     </row>
     <row r="126" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A126" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
     </row>
     <row r="127" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A127" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
     </row>
     <row r="129" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A129" s="8" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="B129" s="8"/>
       <c r="C129" s="8"/>
@@ -2003,7 +2015,7 @@
     </row>
     <row r="130" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A130" s="8" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="B130" s="8"/>
       <c r="C130" s="8"/>
@@ -2011,7 +2023,7 @@
     </row>
     <row r="131" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A131" s="8" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="B131" s="8"/>
       <c r="C131" s="8"/>
@@ -2019,12 +2031,12 @@
     </row>
     <row r="133" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A133" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
     </row>
     <row r="135" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A135" s="8" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="B135" s="8"/>
       <c r="C135" s="8"/>
@@ -2032,17 +2044,17 @@
     </row>
     <row r="136" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A136" s="8" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="B136" s="8" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="C136" s="8"/>
       <c r="D136" s="8"/>
     </row>
     <row r="137" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A137" s="8" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="B137" s="8"/>
       <c r="C137" s="8"/>
@@ -2050,15 +2062,15 @@
     </row>
     <row r="139" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A139" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
     </row>
     <row r="141" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A141" s="8" t="s">
-        <v>174</v>
+        <v>188</v>
       </c>
       <c r="B141" s="8" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="C141" s="8"/>
       <c r="D141" s="8"/>
@@ -2071,52 +2083,55 @@
     </row>
     <row r="143" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A143" s="8" t="s">
-        <v>175</v>
+        <v>189</v>
       </c>
       <c r="B143" s="8" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="C143" s="8"/>
       <c r="D143" s="8"/>
     </row>
     <row r="144" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A144" t="s">
-        <v>176</v>
+        <v>105</v>
       </c>
     </row>
     <row r="145" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A145" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="147" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A147" s="8" t="s">
         <v>107</v>
       </c>
-    </row>
-    <row r="146" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A146" t="s">
+      <c r="B147" s="8" t="s">
+        <v>103</v>
+      </c>
+      <c r="C147" s="8"/>
+      <c r="D147" s="8"/>
+    </row>
+    <row r="149" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A149" t="s">
         <v>108</v>
       </c>
-    </row>
-    <row r="148" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A148" s="8" t="s">
-        <v>109</v>
-      </c>
-      <c r="B148" s="8" t="s">
-        <v>105</v>
-      </c>
-      <c r="C148" s="8"/>
-      <c r="D148" s="8"/>
     </row>
     <row r="150" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A150" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="152" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A152" s="8" t="s">
         <v>110</v>
       </c>
-    </row>
-    <row r="151" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A151" t="s">
-        <v>111</v>
-      </c>
+      <c r="B152" s="8"/>
+      <c r="C152" s="8"/>
+      <c r="D152" s="8"/>
     </row>
     <row r="153" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A153" s="8" t="s">
-        <v>112</v>
+        <v>87</v>
       </c>
       <c r="B153" s="8"/>
       <c r="C153" s="8"/>
@@ -2124,7 +2139,7 @@
     </row>
     <row r="154" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A154" s="8" t="s">
-        <v>89</v>
+        <v>111</v>
       </c>
       <c r="B154" s="8"/>
       <c r="C154" s="8"/>
@@ -2132,29 +2147,29 @@
     </row>
     <row r="155" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A155" s="8" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="B155" s="8"/>
       <c r="C155" s="8"/>
       <c r="D155" s="8"/>
     </row>
     <row r="156" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A156" s="8" t="s">
-        <v>114</v>
-      </c>
+      <c r="A156" s="8"/>
       <c r="B156" s="8"/>
       <c r="C156" s="8"/>
       <c r="D156" s="8"/>
     </row>
     <row r="157" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A157" s="8"/>
+      <c r="A157" s="8" t="s">
+        <v>113</v>
+      </c>
       <c r="B157" s="8"/>
       <c r="C157" s="8"/>
       <c r="D157" s="8"/>
     </row>
     <row r="158" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A158" s="8" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="B158" s="8"/>
       <c r="C158" s="8"/>
@@ -2162,375 +2177,390 @@
     </row>
     <row r="159" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A159" s="8" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="B159" s="8"/>
       <c r="C159" s="8"/>
       <c r="D159" s="8"/>
     </row>
     <row r="160" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A160" s="8" t="s">
-        <v>117</v>
-      </c>
+      <c r="A160" s="8"/>
       <c r="B160" s="8"/>
       <c r="C160" s="8"/>
       <c r="D160" s="8"/>
     </row>
     <row r="161" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A161" s="8"/>
-      <c r="B161" s="8"/>
+      <c r="A161" s="8" t="s">
+        <v>116</v>
+      </c>
+      <c r="B161" s="8" t="s">
+        <v>117</v>
+      </c>
       <c r="C161" s="8"/>
       <c r="D161" s="8"/>
     </row>
     <row r="162" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A162" s="8" t="s">
-        <v>118</v>
-      </c>
-      <c r="B162" s="8" t="s">
-        <v>119</v>
-      </c>
+      <c r="A162" s="8"/>
+      <c r="B162" s="8"/>
       <c r="C162" s="8"/>
       <c r="D162" s="8"/>
     </row>
     <row r="163" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A163" s="8"/>
-      <c r="B163" s="8"/>
+      <c r="A163" s="8" t="s">
+        <v>118</v>
+      </c>
+      <c r="B163" s="8" t="s">
+        <v>88</v>
+      </c>
       <c r="C163" s="8"/>
       <c r="D163" s="8"/>
     </row>
-    <row r="164" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A164" s="8" t="s">
+    <row r="165" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A165" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="167" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A167" s="8" t="s">
         <v>120</v>
       </c>
-      <c r="B164" s="8" t="s">
-        <v>90</v>
-      </c>
-      <c r="C164" s="8"/>
-      <c r="D164" s="8"/>
-    </row>
-    <row r="166" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A166" t="s">
-        <v>121</v>
-      </c>
+      <c r="B167" s="8"/>
+      <c r="C167" s="8"/>
+      <c r="D167" s="8"/>
     </row>
     <row r="168" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A168" s="8" t="s">
-        <v>122</v>
-      </c>
-      <c r="B168" s="8"/>
+        <v>114</v>
+      </c>
+      <c r="B168" s="8" t="s">
+        <v>117</v>
+      </c>
       <c r="C168" s="8"/>
       <c r="D168" s="8"/>
     </row>
     <row r="169" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A169" s="8" t="s">
-        <v>116</v>
+        <v>121</v>
       </c>
       <c r="B169" s="8" t="s">
-        <v>119</v>
+        <v>88</v>
       </c>
       <c r="C169" s="8"/>
       <c r="D169" s="8"/>
     </row>
-    <row r="170" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A170" s="8" t="s">
-        <v>123</v>
-      </c>
-      <c r="B170" s="8" t="s">
-        <v>90</v>
-      </c>
-      <c r="C170" s="8"/>
-      <c r="D170" s="8"/>
+    <row r="171" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A171" t="s">
+        <v>195</v>
+      </c>
     </row>
     <row r="172" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A172" s="16" t="s">
-        <v>152</v>
+      <c r="A172" t="s">
+        <v>196</v>
       </c>
     </row>
     <row r="173" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A173" s="16" t="s">
-        <v>190</v>
-      </c>
-    </row>
-    <row r="174" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A174" s="16" t="s">
-        <v>191</v>
-      </c>
-    </row>
-    <row r="175" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A175" s="8" t="s">
-        <v>185</v>
-      </c>
-      <c r="B175" s="8" t="s">
-        <v>186</v>
-      </c>
-      <c r="C175" s="8"/>
-      <c r="D175" s="8"/>
+      <c r="A173" t="s">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="174" spans="1:4" s="8" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A174" s="8" t="s">
+        <v>194</v>
+      </c>
+      <c r="B174" s="8" t="s">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="176" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A176" s="16" t="s">
+        <v>150</v>
+      </c>
     </row>
     <row r="177" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A177" s="16" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="178" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A178" s="16" t="s">
         <v>192</v>
       </c>
     </row>
     <row r="179" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A179" s="8" t="s">
-        <v>189</v>
+        <v>180</v>
       </c>
       <c r="B179" s="8" t="s">
-        <v>187</v>
+        <v>181</v>
       </c>
       <c r="C179" s="8"/>
       <c r="D179" s="8"/>
     </row>
-    <row r="180" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A180" s="16" t="s">
-        <v>188</v>
-      </c>
-      <c r="B180" s="16"/>
-    </row>
-    <row r="181" spans="1:4" s="16" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="182" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A182" s="16" t="s">
-        <v>193</v>
+    <row r="181" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A181" s="16" t="s">
+        <v>186</v>
       </c>
     </row>
     <row r="183" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A183" s="16" t="s">
-        <v>153</v>
-      </c>
+      <c r="A183" s="8" t="s">
+        <v>184</v>
+      </c>
+      <c r="B183" s="8" t="s">
+        <v>182</v>
+      </c>
+      <c r="C183" s="8"/>
+      <c r="D183" s="8"/>
     </row>
     <row r="184" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A184" s="16" t="s">
-        <v>127</v>
-      </c>
-    </row>
-    <row r="185" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A185" s="16" t="s">
-        <v>130</v>
-      </c>
-    </row>
+        <v>183</v>
+      </c>
+      <c r="B184" s="16"/>
+    </row>
+    <row r="185" spans="1:4" s="16" customFormat="1" x14ac:dyDescent="0.3"/>
     <row r="186" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A186" s="16" t="s">
-        <v>131</v>
+        <v>187</v>
       </c>
     </row>
     <row r="187" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A187" s="16" t="s">
-        <v>132</v>
+        <v>151</v>
       </c>
     </row>
     <row r="188" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A188" s="16" t="s">
-        <v>133</v>
+        <v>125</v>
       </c>
     </row>
     <row r="189" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A189" s="16" t="s">
-        <v>134</v>
+        <v>128</v>
       </c>
     </row>
     <row r="190" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A190" s="16" t="s">
-        <v>135</v>
+        <v>129</v>
       </c>
     </row>
     <row r="191" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A191" s="16" t="s">
-        <v>136</v>
+        <v>130</v>
       </c>
     </row>
     <row r="192" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A192" s="16" t="s">
-        <v>137</v>
+        <v>131</v>
       </c>
     </row>
     <row r="193" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A193" s="16" t="s">
-        <v>139</v>
+        <v>132</v>
       </c>
     </row>
     <row r="194" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A194" s="8" t="s">
-        <v>140</v>
-      </c>
-      <c r="B194" s="8" t="s">
-        <v>141</v>
-      </c>
-      <c r="C194" s="8"/>
-      <c r="D194" s="8"/>
+      <c r="A194" s="16" t="s">
+        <v>133</v>
+      </c>
     </row>
     <row r="195" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A195" s="16" t="s">
-        <v>184</v>
+        <v>134</v>
       </c>
     </row>
     <row r="196" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A196" s="16"/>
+      <c r="A196" s="16" t="s">
+        <v>135</v>
+      </c>
     </row>
     <row r="197" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A197" s="16" t="s">
-        <v>128</v>
+        <v>137</v>
       </c>
     </row>
     <row r="198" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A198" s="16" t="s">
+      <c r="A198" s="8" t="s">
         <v>138</v>
       </c>
+      <c r="B198" s="8" t="s">
+        <v>139</v>
+      </c>
+      <c r="C198" s="8"/>
+      <c r="D198" s="8"/>
     </row>
     <row r="199" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A199" s="8" t="s">
+      <c r="A199" s="16" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="200" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A200" s="16"/>
+    </row>
+    <row r="201" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A201" s="16" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="202" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A202" s="16" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="203" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A203" s="8" t="s">
+        <v>159</v>
+      </c>
+      <c r="B203" s="8" t="s">
+        <v>160</v>
+      </c>
+      <c r="C203" s="8"/>
+      <c r="D203" s="8"/>
+    </row>
+    <row r="204" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A204" s="15"/>
+      <c r="B204" s="15"/>
+      <c r="C204" s="15"/>
+      <c r="D204" s="15"/>
+    </row>
+    <row r="205" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A205" s="15" t="s">
         <v>161</v>
       </c>
-      <c r="B199" s="8" t="s">
+      <c r="B205" s="15" t="s">
         <v>162</v>
       </c>
-      <c r="C199" s="8"/>
-      <c r="D199" s="8"/>
-    </row>
-    <row r="200" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A200" s="15"/>
-      <c r="B200" s="15"/>
-      <c r="C200" s="15"/>
-      <c r="D200" s="15"/>
-    </row>
-    <row r="201" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A201" s="15" t="s">
-        <v>163</v>
-      </c>
-      <c r="B201" s="15" t="s">
-        <v>164</v>
-      </c>
-      <c r="C201" s="15"/>
-      <c r="D201" s="15"/>
-    </row>
-    <row r="202" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A202" s="15"/>
-      <c r="B202" s="15"/>
-      <c r="C202" s="15"/>
-      <c r="D202" s="15"/>
-    </row>
-    <row r="203" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A203" s="16" t="s">
-        <v>129</v>
-      </c>
-    </row>
-    <row r="204" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A204" s="16"/>
-    </row>
-    <row r="205" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A205" s="16" t="s">
-        <v>154</v>
-      </c>
-    </row>
-    <row r="206" spans="1:4" s="17" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A206" s="16" t="s">
-        <v>181</v>
-      </c>
-    </row>
-    <row r="207" spans="1:4" s="17" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="C205" s="15"/>
+      <c r="D205" s="15"/>
+    </row>
+    <row r="206" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A206" s="15"/>
+      <c r="B206" s="15"/>
+      <c r="C206" s="15"/>
+      <c r="D206" s="15"/>
+    </row>
+    <row r="207" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A207" s="16" t="s">
-        <v>142</v>
-      </c>
-    </row>
-    <row r="208" spans="1:4" s="16" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A208" s="15" t="s">
-        <v>143</v>
-      </c>
-      <c r="B208" s="15" t="s">
-        <v>179</v>
-      </c>
-      <c r="C208" s="15"/>
-      <c r="D208" s="15"/>
+        <v>127</v>
+      </c>
+    </row>
+    <row r="208" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A208" s="16"/>
     </row>
     <row r="209" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A209" s="16"/>
-    </row>
-    <row r="210" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A209" s="16" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="210" spans="1:4" s="17" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A210" s="16" t="s">
-        <v>183</v>
-      </c>
-    </row>
-    <row r="211" spans="1:4" x14ac:dyDescent="0.3">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="211" spans="1:4" s="17" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A211" s="16" t="s">
-        <v>180</v>
-      </c>
-    </row>
-    <row r="212" spans="1:4" x14ac:dyDescent="0.3">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="212" spans="1:4" s="16" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A212" s="15" t="s">
-        <v>177</v>
+        <v>141</v>
       </c>
       <c r="B212" s="15" t="s">
-        <v>178</v>
+        <v>174</v>
       </c>
       <c r="C212" s="15"/>
       <c r="D212" s="15"/>
     </row>
     <row r="213" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A213" s="15" t="s">
-        <v>182</v>
-      </c>
-      <c r="B213" s="15"/>
-      <c r="C213" s="15"/>
-      <c r="D213" s="15"/>
+      <c r="A213" s="16"/>
     </row>
     <row r="214" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A214" s="16"/>
+      <c r="A214" s="16" t="s">
+        <v>178</v>
+      </c>
     </row>
     <row r="215" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A215" s="16" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="216" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A216" s="15" t="s">
+        <v>172</v>
+      </c>
+      <c r="B216" s="15" t="s">
+        <v>173</v>
+      </c>
+      <c r="C216" s="15"/>
+      <c r="D216" s="15"/>
+    </row>
+    <row r="217" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A217" s="15" t="s">
+        <v>177</v>
+      </c>
+      <c r="B217" s="15"/>
+      <c r="C217" s="15"/>
+      <c r="D217" s="15"/>
+    </row>
+    <row r="218" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A218" s="16"/>
+    </row>
+    <row r="219" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A219" s="16" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="220" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A220" s="16" t="s">
         <v>144</v>
       </c>
     </row>
-    <row r="216" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A216" s="16" t="s">
+    <row r="221" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A221" s="16" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="222" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A222" s="16" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="223" spans="1:4" s="16" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A223" s="15" t="s">
+        <v>153</v>
+      </c>
+      <c r="B223" s="15" t="s">
         <v>146</v>
       </c>
-    </row>
-    <row r="217" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A217" s="16" t="s">
+      <c r="C223" s="15"/>
+      <c r="D223" s="15"/>
+    </row>
+    <row r="224" spans="1:4" s="16" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A224" s="15"/>
+      <c r="B224" s="15"/>
+      <c r="C224" s="15"/>
+      <c r="D224" s="15"/>
+    </row>
+    <row r="225" spans="1:4" s="16" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A225" s="15" t="s">
         <v>147</v>
       </c>
-    </row>
-    <row r="218" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A218" s="16" t="s">
-        <v>145</v>
-      </c>
-    </row>
-    <row r="219" spans="1:4" s="16" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A219" s="15" t="s">
-        <v>155</v>
-      </c>
-      <c r="B219" s="15" t="s">
+      <c r="B225" s="15"/>
+      <c r="C225" s="15"/>
+      <c r="D225" s="15"/>
+    </row>
+    <row r="226" spans="1:4" s="16" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A226" s="15" t="s">
         <v>148</v>
       </c>
-      <c r="C219" s="15"/>
-      <c r="D219" s="15"/>
-    </row>
-    <row r="220" spans="1:4" s="16" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A220" s="15"/>
-      <c r="B220" s="15"/>
-      <c r="C220" s="15"/>
-      <c r="D220" s="15"/>
-    </row>
-    <row r="221" spans="1:4" s="16" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A221" s="15" t="s">
+      <c r="B226" s="15" t="s">
         <v>149</v>
       </c>
-      <c r="B221" s="15"/>
-      <c r="C221" s="15"/>
-      <c r="D221" s="15"/>
-    </row>
-    <row r="222" spans="1:4" s="16" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A222" s="15" t="s">
-        <v>150</v>
-      </c>
-      <c r="B222" s="15" t="s">
-        <v>151</v>
-      </c>
-      <c r="C222" s="15"/>
-      <c r="D222" s="15"/>
-    </row>
-    <row r="223" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A223" s="16"/>
+      <c r="C226" s="15"/>
+      <c r="D226" s="15"/>
+    </row>
+    <row r="227" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A227" s="16"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Adding examples and documentation about welcome/anything_else/true/false nodes in T2C (in English, Czech is there already)
</commit_message>
<xml_diff>
--- a/example/cz_app/xls/E_CZ_T2C_authoring.xlsx
+++ b/example/cz_app/xls/E_CZ_T2C_authoring.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20827"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B7BFDBBC-C859-4AED-B58C-854CD004EAE6}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4348DCB5-C264-43CA-9E20-E6ED12FE1E7B}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="15336" windowHeight="3744" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="211" uniqueCount="198">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="232" uniqueCount="205">
   <si>
     <r>
       <rPr>
@@ -417,9 +417,6 @@
     <t>// Pokud chcete omezit podmínku, můžete přidat podmínku, že je zároveň rozpoznán i nějaký intent např.</t>
   </si>
   <si>
-    <t>#BOLEST &amp;&amp; @KONCETINA:ruka</t>
-  </si>
-  <si>
     <t>// Podobne lze zapisovat podobný typ otázek. Velmi často se například objevují otázky typu "Co je to  xxx", otázka má řadu variant např. "Vysvětlete mi prosím xxx" a předmět dotazu také. </t>
   </si>
   <si>
@@ -444,19 +441,10 @@
     <t>rentgen;RTG</t>
   </si>
   <si>
-    <t>#CO_JE &amp;&amp; @PREDMET:CT</t>
-  </si>
-  <si>
     <t xml:space="preserve">Počítačová (computerová) tomografie kombinuje klasické rentgenové vyšetřením s počítačovým systémem, který informace zpracovává. </t>
   </si>
   <si>
-    <t>#CO_JE &amp;&amp; @PREDMET:rentgen</t>
-  </si>
-  <si>
     <t>// Pokud má entita velké množství položek, je přehlednější následující formát zápisu</t>
-  </si>
-  <si>
-    <t>#CO_JE &amp;&amp; @PREDMET:&lt;x&gt;</t>
   </si>
   <si>
     <t>rentgen</t>
@@ -831,12 +819,69 @@
   <si>
     <t>// stejne, jak je chápe watson assistant, tedy aby se výstup zobrazil jen po startu konverzace (welcome), vždy (true), nikdy (false) nebo pokud nebyla splněna žádná předchozí podmínka(anything_else).</t>
   </si>
+  <si>
+    <t>#CO_JE and @PREDMET:CT</t>
+  </si>
+  <si>
+    <t>#CO_JE and @PREDMET:rentgen</t>
+  </si>
+  <si>
+    <t>#CO_JE and @PREDMET:&lt;x&gt;</t>
+  </si>
+  <si>
+    <t>#BOLEST and @KONCETINA:ruka</t>
+  </si>
+  <si>
+    <t>#$ anything_else</t>
+  </si>
+  <si>
+    <t>Pardon, nerozumím</t>
+  </si>
+  <si>
+    <t xml:space="preserve">// Je důležité  si stále uvědomovat, že bloky v T2C jsou  prováděny jeden za druhým dokud se najde podmínka, terá je splněna. Výjimkou je, pokud ve sloupci D je uvedeno návěští.   </t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">//  Standardní postup jak to zajistit je ukončit každou větev vyhodnocování pravidlem s podmínkou </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="238"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">#$ anything_else. </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> Takové pravidlo obslouží případy, kdy není splněno žádné z předchozích pravidel.</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">//     pokud se vykonává nějaká lokální větev, je nutné zajistit aby vyhodnocování nepřeteklo do další větve. </t>
+  </si>
+  <si>
+    <t>Jsem rád že souhlasíte</t>
+  </si>
+  <si>
+    <t>To mne mrzí, že nesouhlasíte</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="9" x14ac:knownFonts="1">
+  <fonts count="10" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -903,6 +948,15 @@
     <font>
       <sz val="11"/>
       <color theme="5" tint="-0.249977111117893"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="238"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <charset val="238"/>
@@ -1257,10 +1311,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D227"/>
+  <dimension ref="A1:D250"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A150" workbookViewId="0">
-      <selection activeCell="B172" sqref="B172"/>
+    <sheetView tabSelected="1" topLeftCell="A96" workbookViewId="0">
+      <selection activeCell="B111" sqref="B111"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1282,7 +1336,7 @@
     </row>
     <row r="4" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>166</v>
+        <v>162</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.3">
@@ -1292,7 +1346,7 @@
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>167</v>
+        <v>163</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.3">
@@ -1353,7 +1407,7 @@
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A19" s="1" t="s">
-        <v>168</v>
+        <v>164</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.3">
@@ -1413,7 +1467,7 @@
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
-        <v>169</v>
+        <v>165</v>
       </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.3">
@@ -1530,7 +1584,7 @@
     </row>
     <row r="51" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A51" t="s">
-        <v>190</v>
+        <v>186</v>
       </c>
     </row>
     <row r="52" spans="1:4" x14ac:dyDescent="0.3">
@@ -1551,10 +1605,10 @@
         <v>43</v>
       </c>
       <c r="C55" s="8" t="s">
-        <v>165</v>
+        <v>161</v>
       </c>
       <c r="D55" s="8" t="s">
-        <v>155</v>
+        <v>151</v>
       </c>
     </row>
     <row r="56" spans="1:4" x14ac:dyDescent="0.3">
@@ -1564,42 +1618,38 @@
       <c r="D56" s="8"/>
     </row>
     <row r="57" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A57" s="8" t="s">
-        <v>156</v>
-      </c>
-      <c r="B57" s="8"/>
+      <c r="A57" s="12" t="s">
+        <v>198</v>
+      </c>
+      <c r="B57" s="9" t="s">
+        <v>199</v>
+      </c>
       <c r="C57" s="8"/>
       <c r="D57" s="8"/>
     </row>
     <row r="58" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A58" s="8" t="s">
-        <v>164</v>
-      </c>
-      <c r="B58" s="9" t="s">
-        <v>44</v>
-      </c>
+      <c r="A58" s="8"/>
+      <c r="B58" s="8"/>
       <c r="C58" s="8"/>
       <c r="D58" s="8"/>
     </row>
     <row r="59" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A59" s="8"/>
+      <c r="A59" s="8" t="s">
+        <v>152</v>
+      </c>
       <c r="B59" s="8"/>
       <c r="C59" s="8"/>
       <c r="D59" s="8"/>
     </row>
-    <row r="60" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A60" s="12" t="s">
-        <v>163</v>
+    <row r="60" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A60" s="8" t="s">
+        <v>160</v>
       </c>
       <c r="B60" s="9" t="s">
-        <v>45</v>
-      </c>
-      <c r="C60" s="8" t="s">
-        <v>46</v>
-      </c>
-      <c r="D60" s="8" t="s">
-        <v>157</v>
-      </c>
+        <v>44</v>
+      </c>
+      <c r="C60" s="8"/>
+      <c r="D60" s="8"/>
     </row>
     <row r="61" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A61" s="8"/>
@@ -1607,214 +1657,218 @@
       <c r="C61" s="8"/>
       <c r="D61" s="8"/>
     </row>
-    <row r="62" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A62" s="8" t="s">
-        <v>158</v>
-      </c>
-      <c r="B62" s="8"/>
-      <c r="C62" s="8"/>
-      <c r="D62" s="8"/>
+    <row r="62" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A62" s="12" t="s">
+        <v>159</v>
+      </c>
+      <c r="B62" s="9" t="s">
+        <v>45</v>
+      </c>
+      <c r="C62" s="8" t="s">
+        <v>46</v>
+      </c>
+      <c r="D62" s="8" t="s">
+        <v>153</v>
+      </c>
     </row>
     <row r="63" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A63" s="8" t="s">
-        <v>47</v>
-      </c>
-      <c r="B63" s="8" t="s">
-        <v>48</v>
-      </c>
+      <c r="A63" s="12"/>
+      <c r="B63" s="9"/>
       <c r="C63" s="8"/>
       <c r="D63" s="8"/>
     </row>
     <row r="64" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A64" s="8"/>
-      <c r="B64" s="8"/>
+      <c r="A64" s="12" t="s">
+        <v>198</v>
+      </c>
+      <c r="B64" s="9" t="s">
+        <v>199</v>
+      </c>
       <c r="C64" s="8"/>
       <c r="D64" s="8"/>
     </row>
     <row r="65" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A65" s="8" t="s">
-        <v>49</v>
-      </c>
-      <c r="B65" s="8" t="s">
-        <v>50</v>
-      </c>
+      <c r="A65" s="8"/>
+      <c r="B65" s="8"/>
       <c r="C65" s="8"/>
       <c r="D65" s="8"/>
     </row>
+    <row r="66" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A66" s="8" t="s">
+        <v>154</v>
+      </c>
+      <c r="B66" s="8"/>
+      <c r="C66" s="8"/>
+      <c r="D66" s="8"/>
+    </row>
     <row r="67" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A67" t="s">
-        <v>170</v>
-      </c>
-    </row>
-    <row r="68" spans="1:4" s="17" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A68" s="16" t="s">
-        <v>122</v>
-      </c>
-    </row>
-    <row r="69" spans="1:4" s="17" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A69" s="16" t="s">
-        <v>154</v>
-      </c>
+      <c r="A67" s="8" t="s">
+        <v>47</v>
+      </c>
+      <c r="B67" s="8" t="s">
+        <v>48</v>
+      </c>
+      <c r="C67" s="8"/>
+      <c r="D67" s="8"/>
+    </row>
+    <row r="68" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A68" s="8"/>
+      <c r="B68" s="8"/>
+      <c r="C68" s="8"/>
+      <c r="D68" s="8"/>
+    </row>
+    <row r="69" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A69" s="8" t="s">
+        <v>49</v>
+      </c>
+      <c r="B69" s="8" t="s">
+        <v>50</v>
+      </c>
+      <c r="C69" s="8"/>
+      <c r="D69" s="8"/>
     </row>
     <row r="70" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A70" s="16" t="s">
-        <v>123</v>
-      </c>
+      <c r="A70" s="15"/>
+      <c r="B70" s="15"/>
+      <c r="C70" s="15"/>
+      <c r="D70" s="15"/>
     </row>
     <row r="71" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A71" s="16" t="s">
-        <v>124</v>
-      </c>
-    </row>
-    <row r="72" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A72" s="16"/>
+      <c r="A71" s="12" t="s">
+        <v>198</v>
+      </c>
+      <c r="B71" s="9" t="s">
+        <v>199</v>
+      </c>
+      <c r="C71" s="8"/>
+      <c r="D71" s="8"/>
     </row>
     <row r="73" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A73" s="13" t="s">
+      <c r="A73" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="74" spans="1:4" s="17" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A74" s="16" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="75" spans="1:4" s="17" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A75" s="16" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="76" spans="1:4" s="17" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A76" s="16"/>
+    </row>
+    <row r="77" spans="1:4" s="17" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A77" s="16" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="78" spans="1:4" s="17" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A78" s="16" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="79" spans="1:4" s="17" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A79" s="16" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="80" spans="1:4" s="17" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A80" s="16"/>
+    </row>
+    <row r="81" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A81" s="16" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="82" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A82" s="16" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="83" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A83" s="16"/>
+    </row>
+    <row r="84" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A84" s="13" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="74" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A74" t="s">
+    <row r="85" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A85" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="75" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A75" t="s">
+    <row r="86" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A86" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="76" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A76" t="s">
+    <row r="87" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A87" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="77" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A77" t="s">
+    <row r="88" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A88" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="78" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A78" t="s">
+    <row r="89" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A89" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="80" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A80" s="9" t="s">
+    <row r="91" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A91" s="9" t="s">
         <v>57</v>
       </c>
-      <c r="B80" s="9"/>
-      <c r="C80" s="9"/>
-      <c r="D80" s="9"/>
-    </row>
-    <row r="81" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A81" s="9" t="s">
+      <c r="B91" s="9"/>
+      <c r="C91" s="9"/>
+      <c r="D91" s="9"/>
+    </row>
+    <row r="92" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A92" s="9" t="s">
         <v>58</v>
       </c>
-      <c r="B81" s="9"/>
-      <c r="C81" s="9"/>
-      <c r="D81" s="9"/>
-    </row>
-    <row r="82" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A82" s="9" t="s">
+      <c r="B92" s="9"/>
+      <c r="C92" s="9"/>
+      <c r="D92" s="9"/>
+    </row>
+    <row r="93" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A93" s="9" t="s">
         <v>59</v>
       </c>
-      <c r="B82" s="9"/>
-      <c r="C82" s="9"/>
-      <c r="D82" s="9"/>
-    </row>
-    <row r="83" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A83" s="9" t="s">
+      <c r="B93" s="9"/>
+      <c r="C93" s="9"/>
+      <c r="D93" s="9"/>
+    </row>
+    <row r="94" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A94" s="9" t="s">
         <v>60</v>
       </c>
-      <c r="B83" s="9"/>
-      <c r="C83" s="9"/>
-      <c r="D83" s="9"/>
-    </row>
-    <row r="84" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A84" s="9" t="s">
+      <c r="B94" s="9"/>
+      <c r="C94" s="9"/>
+      <c r="D94" s="9"/>
+    </row>
+    <row r="95" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A95" s="9" t="s">
         <v>61</v>
       </c>
-      <c r="B84" s="9"/>
-      <c r="C84" s="9"/>
-      <c r="D84" s="9"/>
-    </row>
-    <row r="85" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A85" s="9" t="s">
+      <c r="B95" s="9"/>
+      <c r="C95" s="9"/>
+      <c r="D95" s="9"/>
+    </row>
+    <row r="96" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A96" s="9" t="s">
         <v>62</v>
       </c>
-      <c r="B85" s="9"/>
-      <c r="C85" s="9"/>
-      <c r="D85" s="9"/>
-    </row>
-    <row r="86" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A86" s="8"/>
-      <c r="B86" s="8"/>
-      <c r="C86" s="8"/>
-      <c r="D86" s="8"/>
-    </row>
-    <row r="87" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A87" s="8" t="s">
-        <v>63</v>
-      </c>
-      <c r="B87" s="8"/>
-      <c r="C87" s="8"/>
-      <c r="D87" s="8"/>
-    </row>
-    <row r="88" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A88" s="8" t="s">
-        <v>64</v>
-      </c>
-      <c r="B88" s="8"/>
-      <c r="C88" s="8"/>
-      <c r="D88" s="8"/>
-    </row>
-    <row r="89" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A89" s="8" t="s">
-        <v>65</v>
-      </c>
-      <c r="B89" s="8"/>
-      <c r="C89" s="8"/>
-      <c r="D89" s="8"/>
-    </row>
-    <row r="90" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A90" s="8" t="s">
-        <v>66</v>
-      </c>
-      <c r="B90" s="8"/>
-      <c r="C90" s="8"/>
-      <c r="D90" s="8"/>
-    </row>
-    <row r="91" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A91" s="8" t="s">
-        <v>67</v>
-      </c>
-      <c r="B91" s="8"/>
-      <c r="C91" s="8"/>
-      <c r="D91" s="8"/>
-    </row>
-    <row r="92" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A92" s="8" t="s">
-        <v>68</v>
-      </c>
-      <c r="B92" s="8"/>
-      <c r="C92" s="8"/>
-      <c r="D92" s="8"/>
-    </row>
-    <row r="94" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A94" t="s">
-        <v>191</v>
-      </c>
-    </row>
-    <row r="96" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A96" s="8" t="s">
-        <v>57</v>
-      </c>
-      <c r="B96" s="8" t="s">
-        <v>69</v>
-      </c>
-      <c r="C96" s="8"/>
-      <c r="D96" s="8"/>
+      <c r="B96" s="9"/>
+      <c r="C96" s="9"/>
+      <c r="D96" s="9"/>
     </row>
     <row r="97" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A97" s="8"/>
@@ -1826,196 +1880,230 @@
       <c r="A98" s="8" t="s">
         <v>63</v>
       </c>
-      <c r="B98" s="8" t="s">
-        <v>70</v>
-      </c>
+      <c r="B98" s="8"/>
       <c r="C98" s="8"/>
       <c r="D98" s="8"/>
     </row>
+    <row r="99" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A99" s="8" t="s">
+        <v>64</v>
+      </c>
+      <c r="B99" s="8"/>
+      <c r="C99" s="8"/>
+      <c r="D99" s="8"/>
+    </row>
     <row r="100" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A100" t="s">
-        <v>71</v>
-      </c>
+      <c r="A100" s="8" t="s">
+        <v>65</v>
+      </c>
+      <c r="B100" s="8"/>
+      <c r="C100" s="8"/>
+      <c r="D100" s="8"/>
+    </row>
+    <row r="101" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A101" s="8" t="s">
+        <v>66</v>
+      </c>
+      <c r="B101" s="8"/>
+      <c r="C101" s="8"/>
+      <c r="D101" s="8"/>
     </row>
     <row r="102" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A102" s="8" t="s">
-        <v>72</v>
-      </c>
-      <c r="B102" s="8" t="s">
-        <v>73</v>
-      </c>
+        <v>67</v>
+      </c>
+      <c r="B102" s="8"/>
       <c r="C102" s="8"/>
-      <c r="D102" s="8" t="s">
-        <v>74</v>
-      </c>
+      <c r="D102" s="8"/>
     </row>
     <row r="103" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A103" s="8" t="s">
-        <v>75</v>
+        <v>68</v>
       </c>
       <c r="B103" s="8"/>
       <c r="C103" s="8"/>
       <c r="D103" s="8"/>
     </row>
-    <row r="104" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A104" s="8" t="s">
-        <v>76</v>
-      </c>
-      <c r="B104" s="8"/>
-      <c r="C104" s="8"/>
-      <c r="D104" s="8"/>
-    </row>
     <row r="105" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A105" s="8"/>
-      <c r="B105" s="8"/>
-      <c r="C105" s="8"/>
-      <c r="D105" s="8"/>
-    </row>
-    <row r="106" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A106" s="8" t="s">
-        <v>77</v>
-      </c>
-      <c r="B106" s="8"/>
-      <c r="C106" s="8"/>
-      <c r="D106" s="8"/>
+      <c r="A105" t="s">
+        <v>187</v>
+      </c>
     </row>
     <row r="107" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A107" s="8" t="s">
         <v>57</v>
       </c>
       <c r="B107" s="8" t="s">
-        <v>78</v>
+        <v>69</v>
       </c>
       <c r="C107" s="8"/>
-      <c r="D107" s="8" t="s">
-        <v>79</v>
-      </c>
+      <c r="D107" s="8"/>
     </row>
     <row r="108" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A108" s="8"/>
-      <c r="B108" s="8"/>
+      <c r="B108" s="8" t="s">
+        <v>203</v>
+      </c>
       <c r="C108" s="8"/>
       <c r="D108" s="8"/>
     </row>
     <row r="109" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A109" s="8" t="s">
-        <v>63</v>
-      </c>
-      <c r="B109" s="8" t="s">
-        <v>80</v>
-      </c>
+      <c r="A109" s="8"/>
+      <c r="B109" s="8"/>
       <c r="C109" s="8"/>
       <c r="D109" s="8"/>
     </row>
     <row r="110" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A110" s="8"/>
-      <c r="B110" s="8"/>
+      <c r="A110" s="8" t="s">
+        <v>63</v>
+      </c>
+      <c r="B110" s="8" t="s">
+        <v>70</v>
+      </c>
       <c r="C110" s="8"/>
       <c r="D110" s="8"/>
     </row>
     <row r="111" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A111" s="8" t="s">
-        <v>81</v>
-      </c>
-      <c r="B111" s="8"/>
+      <c r="A111" s="8"/>
+      <c r="B111" s="8" t="s">
+        <v>204</v>
+      </c>
       <c r="C111" s="8"/>
       <c r="D111" s="8"/>
     </row>
     <row r="112" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A112" s="8" t="s">
-        <v>57</v>
-      </c>
-      <c r="B112" s="8" t="s">
-        <v>82</v>
-      </c>
+      <c r="A112" s="8"/>
+      <c r="B112" s="8"/>
       <c r="C112" s="8"/>
       <c r="D112" s="8"/>
     </row>
     <row r="113" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A113" s="8"/>
-      <c r="B113" s="8"/>
+      <c r="A113" s="12" t="s">
+        <v>198</v>
+      </c>
+      <c r="B113" s="9" t="s">
+        <v>199</v>
+      </c>
       <c r="C113" s="8"/>
       <c r="D113" s="8"/>
     </row>
-    <row r="114" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A114" s="8" t="s">
-        <v>63</v>
-      </c>
-      <c r="B114" s="8" t="s">
-        <v>83</v>
-      </c>
-      <c r="C114" s="8"/>
-      <c r="D114" s="8"/>
-    </row>
-    <row r="116" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A116" t="s">
-        <v>84</v>
+    <row r="114" spans="1:4" hidden="1" x14ac:dyDescent="0.3"/>
+    <row r="115" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A115" t="s">
+        <v>71</v>
       </c>
     </row>
     <row r="117" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A117" t="s">
-        <v>85</v>
-      </c>
+      <c r="A117" s="8" t="s">
+        <v>72</v>
+      </c>
+      <c r="B117" s="8" t="s">
+        <v>73</v>
+      </c>
+      <c r="C117" s="8"/>
+      <c r="D117" s="8" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="118" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A118" s="8" t="s">
+        <v>75</v>
+      </c>
+      <c r="B118" s="8"/>
+      <c r="C118" s="8"/>
+      <c r="D118" s="8"/>
     </row>
     <row r="119" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A119" t="s">
-        <v>86</v>
-      </c>
+      <c r="A119" s="8" t="s">
+        <v>76</v>
+      </c>
+      <c r="B119" s="8"/>
+      <c r="C119" s="8"/>
+      <c r="D119" s="8"/>
     </row>
     <row r="120" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A120" s="8" t="s">
-        <v>87</v>
-      </c>
-      <c r="B120" s="8" t="s">
-        <v>88</v>
-      </c>
+      <c r="A120" s="8"/>
+      <c r="B120" s="8"/>
       <c r="C120" s="8"/>
       <c r="D120" s="8"/>
     </row>
     <row r="121" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A121" s="8" t="s">
-        <v>89</v>
-      </c>
-      <c r="B121" s="8"/>
+      <c r="A121" s="12" t="s">
+        <v>198</v>
+      </c>
+      <c r="B121" s="9" t="s">
+        <v>199</v>
+      </c>
       <c r="C121" s="8"/>
       <c r="D121" s="8"/>
     </row>
+    <row r="122" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A122" s="8"/>
+      <c r="B122" s="8"/>
+      <c r="C122" s="8"/>
+      <c r="D122" s="8"/>
+    </row>
     <row r="123" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A123" s="13" t="s">
-        <v>90</v>
-      </c>
+      <c r="A123" s="8" t="s">
+        <v>77</v>
+      </c>
+      <c r="B123" s="8"/>
+      <c r="C123" s="8"/>
+      <c r="D123" s="8"/>
     </row>
     <row r="124" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A124" s="14" t="s">
-        <v>91</v>
+      <c r="A124" s="8" t="s">
+        <v>57</v>
+      </c>
+      <c r="B124" s="8" t="s">
+        <v>78</v>
+      </c>
+      <c r="C124" s="8"/>
+      <c r="D124" s="8" t="s">
+        <v>79</v>
       </c>
     </row>
     <row r="125" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A125" t="s">
-        <v>92</v>
-      </c>
+      <c r="A125" s="8"/>
+      <c r="B125" s="8"/>
+      <c r="C125" s="8"/>
+      <c r="D125" s="8"/>
     </row>
     <row r="126" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A126" t="s">
-        <v>93</v>
-      </c>
+      <c r="A126" s="8" t="s">
+        <v>63</v>
+      </c>
+      <c r="B126" s="8" t="s">
+        <v>80</v>
+      </c>
+      <c r="C126" s="8"/>
+      <c r="D126" s="8"/>
     </row>
     <row r="127" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A127" t="s">
-        <v>94</v>
-      </c>
+      <c r="A127" s="8"/>
+      <c r="B127" s="8"/>
+      <c r="C127" s="8"/>
+      <c r="D127" s="8"/>
+    </row>
+    <row r="128" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A128" s="12" t="s">
+        <v>198</v>
+      </c>
+      <c r="B128" s="9" t="s">
+        <v>199</v>
+      </c>
+      <c r="C128" s="8"/>
+      <c r="D128" s="8"/>
     </row>
     <row r="129" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A129" s="8" t="s">
-        <v>171</v>
-      </c>
+      <c r="A129" s="8"/>
       <c r="B129" s="8"/>
       <c r="C129" s="8"/>
       <c r="D129" s="8"/>
     </row>
     <row r="130" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A130" s="8" t="s">
-        <v>95</v>
+        <v>81</v>
       </c>
       <c r="B130" s="8"/>
       <c r="C130" s="8"/>
@@ -2023,544 +2111,676 @@
     </row>
     <row r="131" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A131" s="8" t="s">
-        <v>96</v>
-      </c>
-      <c r="B131" s="8"/>
+        <v>57</v>
+      </c>
+      <c r="B131" s="8" t="s">
+        <v>82</v>
+      </c>
       <c r="C131" s="8"/>
       <c r="D131" s="8"/>
     </row>
+    <row r="132" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A132" s="8"/>
+      <c r="B132" s="8"/>
+      <c r="C132" s="8"/>
+      <c r="D132" s="8"/>
+    </row>
     <row r="133" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A133" t="s">
-        <v>97</v>
-      </c>
+      <c r="A133" s="8" t="s">
+        <v>63</v>
+      </c>
+      <c r="B133" s="8" t="s">
+        <v>83</v>
+      </c>
+      <c r="C133" s="8"/>
+      <c r="D133" s="8"/>
+    </row>
+    <row r="134" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A134" s="8"/>
+      <c r="B134" s="8"/>
+      <c r="C134" s="8"/>
+      <c r="D134" s="8"/>
     </row>
     <row r="135" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A135" s="8" t="s">
-        <v>98</v>
-      </c>
-      <c r="B135" s="8"/>
+      <c r="A135" s="12" t="s">
+        <v>198</v>
+      </c>
+      <c r="B135" s="9" t="s">
+        <v>199</v>
+      </c>
       <c r="C135" s="8"/>
       <c r="D135" s="8"/>
     </row>
-    <row r="136" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A136" s="8" t="s">
-        <v>99</v>
-      </c>
-      <c r="B136" s="8" t="s">
-        <v>100</v>
-      </c>
-      <c r="C136" s="8"/>
-      <c r="D136" s="8"/>
-    </row>
     <row r="137" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A137" s="8" t="s">
-        <v>101</v>
-      </c>
-      <c r="B137" s="8"/>
-      <c r="C137" s="8"/>
-      <c r="D137" s="8"/>
-    </row>
-    <row r="139" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A139" t="s">
-        <v>102</v>
+      <c r="A137" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="138" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A138" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="140" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A140" t="s">
+        <v>86</v>
       </c>
     </row>
     <row r="141" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A141" s="8" t="s">
-        <v>188</v>
+        <v>87</v>
       </c>
       <c r="B141" s="8" t="s">
-        <v>103</v>
+        <v>88</v>
       </c>
       <c r="C141" s="8"/>
       <c r="D141" s="8"/>
     </row>
     <row r="142" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A142" s="8"/>
+      <c r="A142" s="8" t="s">
+        <v>89</v>
+      </c>
       <c r="B142" s="8"/>
       <c r="C142" s="8"/>
       <c r="D142" s="8"/>
     </row>
-    <row r="143" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A143" s="8" t="s">
-        <v>189</v>
-      </c>
-      <c r="B143" s="8" t="s">
-        <v>104</v>
-      </c>
-      <c r="C143" s="8"/>
-      <c r="D143" s="8"/>
-    </row>
     <row r="144" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A144" t="s">
-        <v>105</v>
+      <c r="A144" s="13" t="s">
+        <v>90</v>
       </c>
     </row>
     <row r="145" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A145" t="s">
-        <v>106</v>
+      <c r="A145" s="14" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="146" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A146" t="s">
+        <v>92</v>
       </c>
     </row>
     <row r="147" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A147" s="8" t="s">
-        <v>107</v>
-      </c>
-      <c r="B147" s="8" t="s">
-        <v>103</v>
-      </c>
-      <c r="C147" s="8"/>
-      <c r="D147" s="8"/>
-    </row>
-    <row r="149" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A149" t="s">
-        <v>108</v>
+      <c r="A147" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="148" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A148" t="s">
+        <v>94</v>
       </c>
     </row>
     <row r="150" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A150" t="s">
-        <v>109</v>
-      </c>
+      <c r="A150" s="8" t="s">
+        <v>167</v>
+      </c>
+      <c r="B150" s="8"/>
+      <c r="C150" s="8"/>
+      <c r="D150" s="8"/>
+    </row>
+    <row r="151" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A151" s="8" t="s">
+        <v>95</v>
+      </c>
+      <c r="B151" s="8"/>
+      <c r="C151" s="8"/>
+      <c r="D151" s="8"/>
     </row>
     <row r="152" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A152" s="8" t="s">
-        <v>110</v>
+        <v>96</v>
       </c>
       <c r="B152" s="8"/>
       <c r="C152" s="8"/>
       <c r="D152" s="8"/>
     </row>
-    <row r="153" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A153" s="8" t="s">
-        <v>87</v>
-      </c>
-      <c r="B153" s="8"/>
-      <c r="C153" s="8"/>
-      <c r="D153" s="8"/>
-    </row>
     <row r="154" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A154" s="8" t="s">
-        <v>111</v>
-      </c>
-      <c r="B154" s="8"/>
-      <c r="C154" s="8"/>
-      <c r="D154" s="8"/>
-    </row>
-    <row r="155" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A155" s="8" t="s">
-        <v>112</v>
-      </c>
-      <c r="B155" s="8"/>
-      <c r="C155" s="8"/>
-      <c r="D155" s="8"/>
+      <c r="A154" t="s">
+        <v>97</v>
+      </c>
     </row>
     <row r="156" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A156" s="8"/>
+      <c r="A156" s="8" t="s">
+        <v>98</v>
+      </c>
       <c r="B156" s="8"/>
       <c r="C156" s="8"/>
       <c r="D156" s="8"/>
     </row>
     <row r="157" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A157" s="8" t="s">
-        <v>113</v>
-      </c>
-      <c r="B157" s="8"/>
+        <v>99</v>
+      </c>
+      <c r="B157" s="8" t="s">
+        <v>100</v>
+      </c>
       <c r="C157" s="8"/>
       <c r="D157" s="8"/>
     </row>
     <row r="158" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A158" s="8" t="s">
-        <v>114</v>
+        <v>101</v>
       </c>
       <c r="B158" s="8"/>
       <c r="C158" s="8"/>
       <c r="D158" s="8"/>
     </row>
-    <row r="159" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A159" s="8" t="s">
-        <v>115</v>
-      </c>
-      <c r="B159" s="8"/>
-      <c r="C159" s="8"/>
-      <c r="D159" s="8"/>
-    </row>
     <row r="160" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A160" s="8"/>
-      <c r="B160" s="8"/>
-      <c r="C160" s="8"/>
-      <c r="D160" s="8"/>
-    </row>
-    <row r="161" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A161" s="8" t="s">
-        <v>116</v>
-      </c>
-      <c r="B161" s="8" t="s">
-        <v>117</v>
-      </c>
-      <c r="C161" s="8"/>
-      <c r="D161" s="8"/>
+      <c r="A160" t="s">
+        <v>102</v>
+      </c>
     </row>
     <row r="162" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A162" s="8"/>
-      <c r="B162" s="8"/>
+      <c r="A162" s="8" t="s">
+        <v>184</v>
+      </c>
+      <c r="B162" s="8" t="s">
+        <v>103</v>
+      </c>
       <c r="C162" s="8"/>
       <c r="D162" s="8"/>
     </row>
     <row r="163" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A163" s="8" t="s">
-        <v>118</v>
-      </c>
-      <c r="B163" s="8" t="s">
-        <v>88</v>
-      </c>
+      <c r="A163" s="8"/>
+      <c r="B163" s="8"/>
       <c r="C163" s="8"/>
       <c r="D163" s="8"/>
     </row>
+    <row r="164" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A164" s="8" t="s">
+        <v>185</v>
+      </c>
+      <c r="B164" s="8" t="s">
+        <v>104</v>
+      </c>
+      <c r="C164" s="8"/>
+      <c r="D164" s="8"/>
+    </row>
     <row r="165" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A165" t="s">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="167" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A167" s="8" t="s">
-        <v>120</v>
-      </c>
-      <c r="B167" s="8"/>
-      <c r="C167" s="8"/>
-      <c r="D167" s="8"/>
+        <v>105</v>
+      </c>
+    </row>
+    <row r="166" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A166" t="s">
+        <v>106</v>
+      </c>
     </row>
     <row r="168" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A168" s="8" t="s">
-        <v>114</v>
+        <v>197</v>
       </c>
       <c r="B168" s="8" t="s">
-        <v>117</v>
+        <v>103</v>
       </c>
       <c r="C168" s="8"/>
       <c r="D168" s="8"/>
     </row>
-    <row r="169" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A169" s="8" t="s">
-        <v>121</v>
-      </c>
-      <c r="B169" s="8" t="s">
-        <v>88</v>
-      </c>
-      <c r="C169" s="8"/>
-      <c r="D169" s="8"/>
+    <row r="170" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A170" t="s">
+        <v>107</v>
+      </c>
     </row>
     <row r="171" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A171" t="s">
-        <v>195</v>
-      </c>
-    </row>
-    <row r="172" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A172" t="s">
-        <v>196</v>
+        <v>108</v>
       </c>
     </row>
     <row r="173" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A173" t="s">
-        <v>197</v>
-      </c>
-    </row>
-    <row r="174" spans="1:4" s="8" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A173" s="8" t="s">
+        <v>109</v>
+      </c>
+      <c r="B173" s="8"/>
+      <c r="C173" s="8"/>
+      <c r="D173" s="8"/>
+    </row>
+    <row r="174" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A174" s="8" t="s">
-        <v>194</v>
-      </c>
-      <c r="B174" s="8" t="s">
-        <v>193</v>
-      </c>
+        <v>87</v>
+      </c>
+      <c r="B174" s="8"/>
+      <c r="C174" s="8"/>
+      <c r="D174" s="8"/>
+    </row>
+    <row r="175" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A175" s="8" t="s">
+        <v>110</v>
+      </c>
+      <c r="B175" s="8"/>
+      <c r="C175" s="8"/>
+      <c r="D175" s="8"/>
     </row>
     <row r="176" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A176" s="16" t="s">
-        <v>150</v>
-      </c>
+      <c r="A176" s="8" t="s">
+        <v>111</v>
+      </c>
+      <c r="B176" s="8"/>
+      <c r="C176" s="8"/>
+      <c r="D176" s="8"/>
     </row>
     <row r="177" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A177" s="16" t="s">
-        <v>185</v>
-      </c>
+      <c r="A177" s="8"/>
+      <c r="B177" s="8"/>
+      <c r="C177" s="8"/>
+      <c r="D177" s="8"/>
     </row>
     <row r="178" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A178" s="16" t="s">
-        <v>192</v>
-      </c>
+      <c r="A178" s="8" t="s">
+        <v>112</v>
+      </c>
+      <c r="B178" s="8"/>
+      <c r="C178" s="8"/>
+      <c r="D178" s="8"/>
     </row>
     <row r="179" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A179" s="8" t="s">
-        <v>180</v>
-      </c>
-      <c r="B179" s="8" t="s">
-        <v>181</v>
-      </c>
+        <v>113</v>
+      </c>
+      <c r="B179" s="8"/>
       <c r="C179" s="8"/>
       <c r="D179" s="8"/>
     </row>
+    <row r="180" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A180" s="8" t="s">
+        <v>114</v>
+      </c>
+      <c r="B180" s="8"/>
+      <c r="C180" s="8"/>
+      <c r="D180" s="8"/>
+    </row>
     <row r="181" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A181" s="16" t="s">
-        <v>186</v>
-      </c>
+      <c r="A181" s="8"/>
+      <c r="B181" s="8"/>
+      <c r="C181" s="8"/>
+      <c r="D181" s="8"/>
+    </row>
+    <row r="182" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A182" s="8" t="s">
+        <v>194</v>
+      </c>
+      <c r="B182" s="8" t="s">
+        <v>115</v>
+      </c>
+      <c r="C182" s="8"/>
+      <c r="D182" s="8"/>
     </row>
     <row r="183" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A183" s="8" t="s">
-        <v>184</v>
-      </c>
-      <c r="B183" s="8" t="s">
-        <v>182</v>
-      </c>
+      <c r="A183" s="8"/>
+      <c r="B183" s="8"/>
       <c r="C183" s="8"/>
       <c r="D183" s="8"/>
     </row>
     <row r="184" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A184" s="16" t="s">
-        <v>183</v>
-      </c>
-      <c r="B184" s="16"/>
-    </row>
-    <row r="185" spans="1:4" s="16" customFormat="1" x14ac:dyDescent="0.3"/>
+      <c r="A184" s="8" t="s">
+        <v>195</v>
+      </c>
+      <c r="B184" s="8" t="s">
+        <v>88</v>
+      </c>
+      <c r="C184" s="8"/>
+      <c r="D184" s="8"/>
+    </row>
+    <row r="185" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A185" s="15"/>
+      <c r="B185" s="15"/>
+      <c r="C185" s="15"/>
+      <c r="D185" s="15"/>
+    </row>
     <row r="186" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A186" s="16" t="s">
-        <v>187</v>
-      </c>
-    </row>
-    <row r="187" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A187" s="16" t="s">
-        <v>151</v>
-      </c>
+      <c r="A186" s="12" t="s">
+        <v>198</v>
+      </c>
+      <c r="B186" s="9" t="s">
+        <v>199</v>
+      </c>
+      <c r="C186" s="8"/>
+      <c r="D186" s="8"/>
     </row>
     <row r="188" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A188" s="16" t="s">
-        <v>125</v>
-      </c>
-    </row>
-    <row r="189" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A189" s="16" t="s">
-        <v>128</v>
+      <c r="A188" t="s">
+        <v>116</v>
       </c>
     </row>
     <row r="190" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A190" s="16" t="s">
-        <v>129</v>
-      </c>
+      <c r="A190" s="8" t="s">
+        <v>196</v>
+      </c>
+      <c r="B190" s="8"/>
+      <c r="C190" s="8"/>
+      <c r="D190" s="8"/>
     </row>
     <row r="191" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A191" s="16" t="s">
-        <v>130</v>
-      </c>
+      <c r="A191" s="8" t="s">
+        <v>113</v>
+      </c>
+      <c r="B191" s="8" t="s">
+        <v>115</v>
+      </c>
+      <c r="C191" s="8"/>
+      <c r="D191" s="8"/>
     </row>
     <row r="192" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A192" s="16" t="s">
-        <v>131</v>
-      </c>
-    </row>
-    <row r="193" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A193" s="16" t="s">
-        <v>132</v>
-      </c>
+      <c r="A192" s="8" t="s">
+        <v>117</v>
+      </c>
+      <c r="B192" s="8" t="s">
+        <v>88</v>
+      </c>
+      <c r="C192" s="8"/>
+      <c r="D192" s="8"/>
     </row>
     <row r="194" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A194" s="16" t="s">
-        <v>133</v>
+      <c r="A194" t="s">
+        <v>191</v>
       </c>
     </row>
     <row r="195" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A195" s="16" t="s">
-        <v>134</v>
+      <c r="A195" t="s">
+        <v>192</v>
       </c>
     </row>
     <row r="196" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A196" s="16" t="s">
-        <v>135</v>
-      </c>
-    </row>
-    <row r="197" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A197" s="16" t="s">
-        <v>137</v>
-      </c>
-    </row>
-    <row r="198" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A198" s="8" t="s">
-        <v>138</v>
-      </c>
-      <c r="B198" s="8" t="s">
-        <v>139</v>
-      </c>
-      <c r="C198" s="8"/>
-      <c r="D198" s="8"/>
+      <c r="A196" t="s">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="197" spans="1:4" s="8" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A197" s="8" t="s">
+        <v>190</v>
+      </c>
+      <c r="B197" s="8" t="s">
+        <v>189</v>
+      </c>
     </row>
     <row r="199" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A199" s="16" t="s">
-        <v>179</v>
+        <v>146</v>
       </c>
     </row>
     <row r="200" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A200" s="16"/>
+      <c r="A200" s="16" t="s">
+        <v>181</v>
+      </c>
     </row>
     <row r="201" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A201" s="16" t="s">
-        <v>126</v>
+        <v>188</v>
       </c>
     </row>
     <row r="202" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A202" s="16" t="s">
-        <v>136</v>
-      </c>
-    </row>
-    <row r="203" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A203" s="8" t="s">
-        <v>159</v>
-      </c>
-      <c r="B203" s="8" t="s">
-        <v>160</v>
-      </c>
-      <c r="C203" s="8"/>
-      <c r="D203" s="8"/>
+      <c r="A202" s="8" t="s">
+        <v>176</v>
+      </c>
+      <c r="B202" s="8" t="s">
+        <v>177</v>
+      </c>
+      <c r="C202" s="8"/>
+      <c r="D202" s="8"/>
     </row>
     <row r="204" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A204" s="15"/>
-      <c r="B204" s="15"/>
-      <c r="C204" s="15"/>
-      <c r="D204" s="15"/>
-    </row>
-    <row r="205" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A205" s="15" t="s">
-        <v>161</v>
-      </c>
-      <c r="B205" s="15" t="s">
-        <v>162</v>
-      </c>
-      <c r="C205" s="15"/>
-      <c r="D205" s="15"/>
+      <c r="A204" s="16" t="s">
+        <v>182</v>
+      </c>
     </row>
     <row r="206" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A206" s="15"/>
-      <c r="B206" s="15"/>
-      <c r="C206" s="15"/>
-      <c r="D206" s="15"/>
+      <c r="A206" s="8" t="s">
+        <v>180</v>
+      </c>
+      <c r="B206" s="8" t="s">
+        <v>178</v>
+      </c>
+      <c r="C206" s="8"/>
+      <c r="D206" s="8"/>
     </row>
     <row r="207" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A207" s="16" t="s">
-        <v>127</v>
-      </c>
-    </row>
-    <row r="208" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A208" s="16"/>
-    </row>
+        <v>179</v>
+      </c>
+      <c r="B207" s="16"/>
+    </row>
+    <row r="208" spans="1:4" s="16" customFormat="1" x14ac:dyDescent="0.3"/>
     <row r="209" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A209" s="16" t="s">
-        <v>152</v>
-      </c>
-    </row>
-    <row r="210" spans="1:4" s="17" customFormat="1" x14ac:dyDescent="0.3">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="210" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A210" s="16" t="s">
-        <v>176</v>
-      </c>
-    </row>
-    <row r="211" spans="1:4" s="17" customFormat="1" x14ac:dyDescent="0.3">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="211" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A211" s="16" t="s">
-        <v>140</v>
-      </c>
-    </row>
-    <row r="212" spans="1:4" s="16" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A212" s="15" t="s">
-        <v>141</v>
-      </c>
-      <c r="B212" s="15" t="s">
-        <v>174</v>
-      </c>
-      <c r="C212" s="15"/>
-      <c r="D212" s="15"/>
+        <v>121</v>
+      </c>
+    </row>
+    <row r="212" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A212" s="16" t="s">
+        <v>124</v>
+      </c>
     </row>
     <row r="213" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A213" s="16"/>
+      <c r="A213" s="16" t="s">
+        <v>125</v>
+      </c>
     </row>
     <row r="214" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A214" s="16" t="s">
-        <v>178</v>
+        <v>126</v>
       </c>
     </row>
     <row r="215" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A215" s="16" t="s">
-        <v>175</v>
+        <v>127</v>
       </c>
     </row>
     <row r="216" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A216" s="15" t="s">
-        <v>172</v>
-      </c>
-      <c r="B216" s="15" t="s">
-        <v>173</v>
-      </c>
-      <c r="C216" s="15"/>
-      <c r="D216" s="15"/>
+      <c r="A216" s="16" t="s">
+        <v>128</v>
+      </c>
     </row>
     <row r="217" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A217" s="15" t="s">
-        <v>177</v>
-      </c>
-      <c r="B217" s="15"/>
-      <c r="C217" s="15"/>
-      <c r="D217" s="15"/>
+      <c r="A217" s="16" t="s">
+        <v>129</v>
+      </c>
     </row>
     <row r="218" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A218" s="16"/>
+      <c r="A218" s="16" t="s">
+        <v>130</v>
+      </c>
     </row>
     <row r="219" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A219" s="16" t="s">
-        <v>142</v>
+        <v>131</v>
       </c>
     </row>
     <row r="220" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A220" s="16" t="s">
-        <v>144</v>
+        <v>133</v>
       </c>
     </row>
     <row r="221" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A221" s="16" t="s">
-        <v>145</v>
-      </c>
+      <c r="A221" s="8" t="s">
+        <v>134</v>
+      </c>
+      <c r="B221" s="8" t="s">
+        <v>135</v>
+      </c>
+      <c r="C221" s="8"/>
+      <c r="D221" s="8"/>
     </row>
     <row r="222" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A222" s="16" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="223" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A223" s="16"/>
+    </row>
+    <row r="224" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A224" s="16" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="225" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A225" s="16" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="226" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A226" s="8" t="s">
+        <v>155</v>
+      </c>
+      <c r="B226" s="8" t="s">
+        <v>156</v>
+      </c>
+      <c r="C226" s="8"/>
+      <c r="D226" s="8"/>
+    </row>
+    <row r="227" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A227" s="15"/>
+      <c r="B227" s="15"/>
+      <c r="C227" s="15"/>
+      <c r="D227" s="15"/>
+    </row>
+    <row r="228" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A228" s="15" t="s">
+        <v>157</v>
+      </c>
+      <c r="B228" s="15" t="s">
+        <v>158</v>
+      </c>
+      <c r="C228" s="15"/>
+      <c r="D228" s="15"/>
+    </row>
+    <row r="229" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A229" s="15"/>
+      <c r="B229" s="15"/>
+      <c r="C229" s="15"/>
+      <c r="D229" s="15"/>
+    </row>
+    <row r="230" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A230" s="16" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="231" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A231" s="16"/>
+    </row>
+    <row r="232" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A232" s="16" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="233" spans="1:4" s="17" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A233" s="16" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="234" spans="1:4" s="17" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A234" s="16" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="235" spans="1:4" s="16" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A235" s="15" t="s">
+        <v>137</v>
+      </c>
+      <c r="B235" s="15" t="s">
+        <v>170</v>
+      </c>
+      <c r="C235" s="15"/>
+      <c r="D235" s="15"/>
+    </row>
+    <row r="236" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A236" s="16"/>
+    </row>
+    <row r="237" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A237" s="16" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="238" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A238" s="16" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="239" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A239" s="15" t="s">
+        <v>168</v>
+      </c>
+      <c r="B239" s="15" t="s">
+        <v>169</v>
+      </c>
+      <c r="C239" s="15"/>
+      <c r="D239" s="15"/>
+    </row>
+    <row r="240" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A240" s="15" t="s">
+        <v>173</v>
+      </c>
+      <c r="B240" s="15"/>
+      <c r="C240" s="15"/>
+      <c r="D240" s="15"/>
+    </row>
+    <row r="241" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A241" s="16"/>
+    </row>
+    <row r="242" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A242" s="16" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="243" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A243" s="16" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="244" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A244" s="16" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="245" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A245" s="16" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="246" spans="1:4" s="16" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A246" s="15" t="s">
+        <v>149</v>
+      </c>
+      <c r="B246" s="15" t="s">
+        <v>142</v>
+      </c>
+      <c r="C246" s="15"/>
+      <c r="D246" s="15"/>
+    </row>
+    <row r="247" spans="1:4" s="16" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A247" s="15"/>
+      <c r="B247" s="15"/>
+      <c r="C247" s="15"/>
+      <c r="D247" s="15"/>
+    </row>
+    <row r="248" spans="1:4" s="16" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A248" s="15" t="s">
         <v>143</v>
       </c>
-    </row>
-    <row r="223" spans="1:4" s="16" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A223" s="15" t="s">
-        <v>153</v>
-      </c>
-      <c r="B223" s="15" t="s">
-        <v>146</v>
-      </c>
-      <c r="C223" s="15"/>
-      <c r="D223" s="15"/>
-    </row>
-    <row r="224" spans="1:4" s="16" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A224" s="15"/>
-      <c r="B224" s="15"/>
-      <c r="C224" s="15"/>
-      <c r="D224" s="15"/>
-    </row>
-    <row r="225" spans="1:4" s="16" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A225" s="15" t="s">
-        <v>147</v>
-      </c>
-      <c r="B225" s="15"/>
-      <c r="C225" s="15"/>
-      <c r="D225" s="15"/>
-    </row>
-    <row r="226" spans="1:4" s="16" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A226" s="15" t="s">
-        <v>148</v>
-      </c>
-      <c r="B226" s="15" t="s">
-        <v>149</v>
-      </c>
-      <c r="C226" s="15"/>
-      <c r="D226" s="15"/>
-    </row>
-    <row r="227" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A227" s="16"/>
+      <c r="B248" s="15"/>
+      <c r="C248" s="15"/>
+      <c r="D248" s="15"/>
+    </row>
+    <row r="249" spans="1:4" s="16" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A249" s="15" t="s">
+        <v>144</v>
+      </c>
+      <c r="B249" s="15" t="s">
+        <v>145</v>
+      </c>
+      <c r="C249" s="15"/>
+      <c r="D249" s="15"/>
+    </row>
+    <row r="250" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A250" s="16"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>